<commit_message>
renamed PIDEncoderSource, will use for all wheel PID.
</commit_message>
<xml_diff>
--- a/SinPathGenerator.xlsx
+++ b/SinPathGenerator.xlsx
@@ -13618,8 +13618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="C315" sqref="C315"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed formatting error in path generator
</commit_message>
<xml_diff>
--- a/SinPathGenerator.xlsx
+++ b/SinPathGenerator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5821,11 +5820,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="19705888"/>
-        <c:axId val="19715712"/>
+        <c:axId val="-1341685856"/>
+        <c:axId val="-1341694048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19705888"/>
+        <c:axId val="-1341685856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +5867,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19715712"/>
+        <c:crossAx val="-1341694048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5876,7 +5875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19715712"/>
+        <c:axId val="-1341694048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5896,6 +5895,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5926,7 +5926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19705888"/>
+        <c:crossAx val="-1341685856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5940,7 +5940,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13619,7 +13618,7 @@
   <dimension ref="A1:C445"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13646,8 +13645,8 @@
         <v>{0,</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(Sheet1!F10=0,","&amp;Sheet1!C10&amp;",","")</f>
-        <v>,0,</v>
+        <f>IF(Sheet1!F10=0,Sheet1!C10&amp;",","")</f>
+        <v>0,</v>
       </c>
       <c r="C3" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D10&amp;"},","}}")</f>
@@ -13660,8 +13659,8 @@
         <v>{0.05,</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(Sheet1!F11=0,","&amp;Sheet1!C11&amp;",","")</f>
-        <v>,0.381278906725964,</v>
+        <f>IF(Sheet1!F11=0,Sheet1!C11&amp;",","")</f>
+        <v>0.381278906725964,</v>
       </c>
       <c r="C4" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D11&amp;"},","}}")</f>
@@ -13674,8 +13673,8 @@
         <v>{0.1,</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(Sheet1!F12=0,","&amp;Sheet1!C12&amp;",","")</f>
-        <v>,0.762003332970849,</v>
+        <f>IF(Sheet1!F12=0,Sheet1!C12&amp;",","")</f>
+        <v>0.762003332970849,</v>
       </c>
       <c r="C5" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D12&amp;"},","}}")</f>
@@ -13688,8 +13687,8 @@
         <v>{0.15,</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(Sheet1!F13=0,","&amp;Sheet1!C13&amp;",","")</f>
-        <v>,1.141619604615,</v>
+        <f>IF(Sheet1!F13=0,Sheet1!C13&amp;",","")</f>
+        <v>1.141619604615,</v>
       </c>
       <c r="C6" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D13&amp;"},","}}")</f>
@@ -13702,8 +13701,8 @@
         <v>{0.2,</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(Sheet1!F14=0,","&amp;Sheet1!C14&amp;",","")</f>
-        <v>,1.51957565908897,</v>
+        <f>IF(Sheet1!F14=0,Sheet1!C14&amp;",","")</f>
+        <v>1.51957565908897,</v>
       </c>
       <c r="C7" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D14&amp;"},","}}")</f>
@@ -13716,8 +13715,8 @@
         <v>{0.25,</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(Sheet1!F15=0,","&amp;Sheet1!C15&amp;",","")</f>
-        <v>,1.89532184821863,</v>
+        <f>IF(Sheet1!F15=0,Sheet1!C15&amp;",","")</f>
+        <v>1.89532184821863,</v>
       </c>
       <c r="C8" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D15&amp;"},","}}")</f>
@@ -13730,8 +13729,8 @@
         <v>{0.3,</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(Sheet1!F16=0,","&amp;Sheet1!C16&amp;",","")</f>
-        <v>,2.26831173755919,</v>
+        <f>IF(Sheet1!F16=0,Sheet1!C16&amp;",","")</f>
+        <v>2.26831173755919,</v>
       </c>
       <c r="C9" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D16&amp;"},","}}")</f>
@@ -13744,8 +13743,8 @@
         <v>{0.35,</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(Sheet1!F17=0,","&amp;Sheet1!C17&amp;",","")</f>
-        <v>,2.6380029010555,</v>
+        <f>IF(Sheet1!F17=0,Sheet1!C17&amp;",","")</f>
+        <v>2.6380029010555,</v>
       </c>
       <c r="C10" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D17&amp;"},","}}")</f>
@@ -13758,8 +13757,8 @@
         <v>{0.4,</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(Sheet1!F18=0,","&amp;Sheet1!C18&amp;",","")</f>
-        <v>,3.00385770987323,</v>
+        <f>IF(Sheet1!F18=0,Sheet1!C18&amp;",","")</f>
+        <v>3.00385770987323,</v>
       </c>
       <c r="C11" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D18&amp;"},","}}")</f>
@@ -13772,8 +13771,8 @@
         <v>{0.45,</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(Sheet1!F19=0,","&amp;Sheet1!C19&amp;",","")</f>
-        <v>,3.36534411425346,</v>
+        <f>IF(Sheet1!F19=0,Sheet1!C19&amp;",","")</f>
+        <v>3.36534411425346,</v>
       </c>
       <c r="C12" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D19&amp;"},","}}")</f>
@@ -13786,8 +13785,8 @@
         <v>{0.5,</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(Sheet1!F20=0,","&amp;Sheet1!C20&amp;",","")</f>
-        <v>,3.72193641725396,</v>
+        <f>IF(Sheet1!F20=0,Sheet1!C20&amp;",","")</f>
+        <v>3.72193641725396,</v>
       </c>
       <c r="C13" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D20&amp;"},","}}")</f>
@@ -13800,8 +13799,8 @@
         <v>{0.55,</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(Sheet1!F21=0,","&amp;Sheet1!C21&amp;",","")</f>
-        <v>,4.07311603925171,</v>
+        <f>IF(Sheet1!F21=0,Sheet1!C21&amp;",","")</f>
+        <v>4.07311603925171,</v>
       </c>
       <c r="C14" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D21&amp;"},","}}")</f>
@@ -13814,8 +13813,8 @@
         <v>{0.6,</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(Sheet1!F22=0,","&amp;Sheet1!C22&amp;",","")</f>
-        <v>,4.41837227209498,</v>
+        <f>IF(Sheet1!F22=0,Sheet1!C22&amp;",","")</f>
+        <v>4.41837227209498,</v>
       </c>
       <c r="C15" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D22&amp;"},","}}")</f>
@@ -13828,8 +13827,8 @@
         <v>{0.65,</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(Sheet1!F23=0,","&amp;Sheet1!C23&amp;",","")</f>
-        <v>,4.75720302180817,</v>
+        <f>IF(Sheet1!F23=0,Sheet1!C23&amp;",","")</f>
+        <v>4.75720302180817,</v>
       </c>
       <c r="C16" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D23&amp;"},","}}")</f>
@@ -13842,8 +13841,8 @@
         <v>{0.7,</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(Sheet1!F24=0,","&amp;Sheet1!C24&amp;",","")</f>
-        <v>,5.08911553876945,</v>
+        <f>IF(Sheet1!F24=0,Sheet1!C24&amp;",","")</f>
+        <v>5.08911553876945,</v>
       </c>
       <c r="C17" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D24&amp;"},","}}")</f>
@@ -13856,8 +13855,8 @@
         <v>{0.75,</v>
       </c>
       <c r="B18" t="str">
-        <f>IF(Sheet1!F25=0,","&amp;Sheet1!C25&amp;",","")</f>
-        <v>,5.41362713429913,</v>
+        <f>IF(Sheet1!F25=0,Sheet1!C25&amp;",","")</f>
+        <v>5.41362713429913,</v>
       </c>
       <c r="C18" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D25&amp;"},","}}")</f>
@@ -13870,8 +13869,8 @@
         <v>{0.8,</v>
       </c>
       <c r="B19" t="str">
-        <f>IF(Sheet1!F26=0,","&amp;Sheet1!C26&amp;",","")</f>
-        <v>,5.73026588261682,</v>
+        <f>IF(Sheet1!F26=0,Sheet1!C26&amp;",","")</f>
+        <v>5.73026588261682,</v>
       </c>
       <c r="C19" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D26&amp;"},","}}")</f>
@@ -13884,8 +13883,8 @@
         <v>{0.85,</v>
       </c>
       <c r="B20" t="str">
-        <f>IF(Sheet1!F27=0,","&amp;Sheet1!C27&amp;",","")</f>
-        <v>,6.03857130714644,</v>
+        <f>IF(Sheet1!F27=0,Sheet1!C27&amp;",","")</f>
+        <v>6.03857130714644,</v>
       </c>
       <c r="C20" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D27&amp;"},","}}")</f>
@@ -13898,8 +13897,8 @@
         <v>{0.9,</v>
       </c>
       <c r="B21" t="str">
-        <f>IF(Sheet1!F28=0,","&amp;Sheet1!C28&amp;",","")</f>
-        <v>,6.33809505017112,</v>
+        <f>IF(Sheet1!F28=0,Sheet1!C28&amp;",","")</f>
+        <v>6.33809505017112,</v>
       </c>
       <c r="C21" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D28&amp;"},","}}")</f>
@@ -13912,8 +13911,8 @@
         <v>{0.95,</v>
       </c>
       <c r="B22" t="str">
-        <f>IF(Sheet1!F29=0,","&amp;Sheet1!C29&amp;",","")</f>
-        <v>,6.62840152486401,</v>
+        <f>IF(Sheet1!F29=0,Sheet1!C29&amp;",","")</f>
+        <v>6.62840152486401,</v>
       </c>
       <c r="C22" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D29&amp;"},","}}")</f>
@@ -13926,8 +13925,8 @@
         <v>{1,</v>
       </c>
       <c r="B23" t="str">
-        <f>IF(Sheet1!F30=0,","&amp;Sheet1!C30&amp;",","")</f>
-        <v>,6.90906854874686,</v>
+        <f>IF(Sheet1!F30=0,Sheet1!C30&amp;",","")</f>
+        <v>6.90906854874686,</v>
       </c>
       <c r="C23" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D30&amp;"},","}}")</f>
@@ -13940,8 +13939,8 @@
         <v>{1.05,</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(Sheet1!F31=0,","&amp;Sheet1!C31&amp;",","")</f>
-        <v>,7.1796879576551,</v>
+        <f>IF(Sheet1!F31=0,Sheet1!C31&amp;",","")</f>
+        <v>7.1796879576551,</v>
       </c>
       <c r="C24" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D31&amp;"},","}}")</f>
@@ -13954,8 +13953,8 @@
         <v>{1.1,</v>
       </c>
       <c r="B25" t="str">
-        <f>IF(Sheet1!F32=0,","&amp;Sheet1!C32&amp;",","")</f>
-        <v>,7.43986619931665,</v>
+        <f>IF(Sheet1!F32=0,Sheet1!C32&amp;",","")</f>
+        <v>7.43986619931665,</v>
       </c>
       <c r="C25" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D32&amp;"},","}}")</f>
@@ -13968,8 +13967,8 @@
         <v>{1.15,</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(Sheet1!F33=0,","&amp;Sheet1!C33&amp;",","")</f>
-        <v>,7.6892249056811,</v>
+        <f>IF(Sheet1!F33=0,Sheet1!C33&amp;",","")</f>
+        <v>7.6892249056811,</v>
       </c>
       <c r="C26" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D33&amp;"},","}}")</f>
@@ -13982,8 +13981,8 @@
         <v>{1.2,</v>
       </c>
       <c r="B27" t="str">
-        <f>IF(Sheet1!F34=0,","&amp;Sheet1!C34&amp;",","")</f>
-        <v>,7.92740144316703,</v>
+        <f>IF(Sheet1!F34=0,Sheet1!C34&amp;",","")</f>
+        <v>7.92740144316703,</v>
       </c>
       <c r="C27" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D34&amp;"},","}}")</f>
@@ -13996,8 +13995,8 @@
         <v>{1.25,</v>
       </c>
       <c r="B28" t="str">
-        <f>IF(Sheet1!F35=0,","&amp;Sheet1!C35&amp;",","")</f>
-        <v>,8.15404944002724,</v>
+        <f>IF(Sheet1!F35=0,Sheet1!C35&amp;",","")</f>
+        <v>8.15404944002724,</v>
       </c>
       <c r="C28" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D35&amp;"},","}}")</f>
@@ -14010,8 +14009,8 @@
         <v>{1.3,</v>
       </c>
       <c r="B29" t="str">
-        <f>IF(Sheet1!F36=0,","&amp;Sheet1!C36&amp;",","")</f>
-        <v>,8.36883929006503,</v>
+        <f>IF(Sheet1!F36=0,Sheet1!C36&amp;",","")</f>
+        <v>8.36883929006503,</v>
       </c>
       <c r="C29" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D36&amp;"},","}}")</f>
@@ -14024,8 +14023,8 @@
         <v>{1.35,</v>
       </c>
       <c r="B30" t="str">
-        <f>IF(Sheet1!F37=0,","&amp;Sheet1!C37&amp;",","")</f>
-        <v>,8.57145863196881,</v>
+        <f>IF(Sheet1!F37=0,Sheet1!C37&amp;",","")</f>
+        <v>8.57145863196881,</v>
       </c>
       <c r="C30" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D37&amp;"},","}}")</f>
@@ -14038,8 +14037,8 @@
         <v>{1.4,</v>
       </c>
       <c r="B31" t="str">
-        <f>IF(Sheet1!F38=0,","&amp;Sheet1!C38&amp;",","")</f>
-        <v>,8.76161280356822,</v>
+        <f>IF(Sheet1!F38=0,Sheet1!C38&amp;",","")</f>
+        <v>8.76161280356822,</v>
       </c>
       <c r="C31" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D38&amp;"},","}}")</f>
@@ -14052,8 +14051,8 @@
         <v>{1.45,</v>
       </c>
       <c r="B32" t="str">
-        <f>IF(Sheet1!F39=0,","&amp;Sheet1!C39&amp;",","")</f>
-        <v>,8.93902527035088,</v>
+        <f>IF(Sheet1!F39=0,Sheet1!C39&amp;",","")</f>
+        <v>8.93902527035088,</v>
       </c>
       <c r="C32" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D39&amp;"},","}}")</f>
@@ -14066,8 +14065,8 @@
         <v>{1.5,</v>
       </c>
       <c r="B33" t="str">
-        <f>IF(Sheet1!F40=0,","&amp;Sheet1!C40&amp;",","")</f>
-        <v>,9.10343802761684,</v>
+        <f>IF(Sheet1!F40=0,Sheet1!C40&amp;",","")</f>
+        <v>9.10343802761684,</v>
       </c>
       <c r="C33" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D40&amp;"},","}}")</f>
@@ -14080,8 +14079,8 @@
         <v>{1.55,</v>
       </c>
       <c r="B34" t="str">
-        <f>IF(Sheet1!F41=0,","&amp;Sheet1!C41&amp;",","")</f>
-        <v>,9.25461197568569,</v>
+        <f>IF(Sheet1!F41=0,Sheet1!C41&amp;",","")</f>
+        <v>9.25461197568569,</v>
       </c>
       <c r="C34" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D41&amp;"},","}}")</f>
@@ -14094,8 +14093,8 @@
         <v>{1.6,</v>
       </c>
       <c r="B35" t="str">
-        <f>IF(Sheet1!F42=0,","&amp;Sheet1!C42&amp;",","")</f>
-        <v>,9.3923272676108,</v>
+        <f>IF(Sheet1!F42=0,Sheet1!C42&amp;",","")</f>
+        <v>9.3923272676108,</v>
       </c>
       <c r="C35" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D42&amp;"},","}}")</f>
@@ -14108,8 +14107,8 @@
         <v>{1.65,</v>
       </c>
       <c r="B36" t="str">
-        <f>IF(Sheet1!F43=0,","&amp;Sheet1!C43&amp;",","")</f>
-        <v>,9.51638362889504,</v>
+        <f>IF(Sheet1!F43=0,Sheet1!C43&amp;",","")</f>
+        <v>9.51638362889504,</v>
       </c>
       <c r="C36" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D43&amp;"},","}}")</f>
@@ -14122,8 +14121,8 @@
         <v>{1.7,</v>
       </c>
       <c r="B37" t="str">
-        <f>IF(Sheet1!F44=0,","&amp;Sheet1!C44&amp;",","")</f>
-        <v>,9.62660064874286,</v>
+        <f>IF(Sheet1!F44=0,Sheet1!C44&amp;",","")</f>
+        <v>9.62660064874286,</v>
       </c>
       <c r="C37" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D44&amp;"},","}}")</f>
@@ -14136,8 +14135,8 @@
         <v>{1.75,</v>
       </c>
       <c r="B38" t="str">
-        <f>IF(Sheet1!F45=0,","&amp;Sheet1!C45&amp;",","")</f>
-        <v>,9.72281804242539,</v>
+        <f>IF(Sheet1!F45=0,Sheet1!C45&amp;",","")</f>
+        <v>9.72281804242539,</v>
       </c>
       <c r="C38" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D45&amp;"},","}}")</f>
@@ -14150,8 +14149,8 @@
         <v>{1.8,</v>
       </c>
       <c r="B39" t="str">
-        <f>IF(Sheet1!F46=0,","&amp;Sheet1!C46&amp;",","")</f>
-        <v>,9.80489588437687,</v>
+        <f>IF(Sheet1!F46=0,Sheet1!C46&amp;",","")</f>
+        <v>9.80489588437687,</v>
       </c>
       <c r="C39" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D46&amp;"},","}}")</f>
@@ -14164,8 +14163,8 @@
         <v>{1.85,</v>
       </c>
       <c r="B40" t="str">
-        <f>IF(Sheet1!F47=0,","&amp;Sheet1!C47&amp;",","")</f>
-        <v>,9.87271481168346,</v>
+        <f>IF(Sheet1!F47=0,Sheet1!C47&amp;",","")</f>
+        <v>9.87271481168346,</v>
       </c>
       <c r="C40" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D47&amp;"},","}}")</f>
@@ -14178,8 +14177,8 @@
         <v>{1.9,</v>
       </c>
       <c r="B41" t="str">
-        <f>IF(Sheet1!F48=0,","&amp;Sheet1!C48&amp;",","")</f>
-        <v>,9.92617619766853,</v>
+        <f>IF(Sheet1!F48=0,Sheet1!C48&amp;",","")</f>
+        <v>9.92617619766853,</v>
       </c>
       <c r="C41" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D48&amp;"},","}}")</f>
@@ -14192,8 +14191,8 @@
         <v>{1.95,</v>
       </c>
       <c r="B42" t="str">
-        <f>IF(Sheet1!F49=0,","&amp;Sheet1!C49&amp;",","")</f>
-        <v>,9.96520229532196,</v>
+        <f>IF(Sheet1!F49=0,Sheet1!C49&amp;",","")</f>
+        <v>9.96520229532196,</v>
       </c>
       <c r="C42" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D49&amp;"},","}}")</f>
@@ -14206,8 +14205,8 @@
         <v>{2,</v>
       </c>
       <c r="B43" t="str">
-        <f>IF(Sheet1!F50=0,","&amp;Sheet1!C50&amp;",","")</f>
-        <v>,9.98973635036487,</v>
+        <f>IF(Sheet1!F50=0,Sheet1!C50&amp;",","")</f>
+        <v>9.98973635036487,</v>
       </c>
       <c r="C43" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D50&amp;"},","}}")</f>
@@ -14220,8 +14219,8 @@
         <v>{2.05,</v>
       </c>
       <c r="B44" t="str">
-        <f>IF(Sheet1!F51=0,","&amp;Sheet1!C51&amp;",","")</f>
-        <v>,9.99974268378539,</v>
+        <f>IF(Sheet1!F51=0,Sheet1!C51&amp;",","")</f>
+        <v>9.99974268378539,</v>
       </c>
       <c r="C44" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D51&amp;"},","}}")</f>
@@ -14234,8 +14233,8 @@
         <v>{2.1,</v>
       </c>
       <c r="B45" t="str">
-        <f>IF(Sheet1!F52=0,","&amp;Sheet1!C52&amp;",","")</f>
-        <v>,9.99520674372535,</v>
+        <f>IF(Sheet1!F52=0,Sheet1!C52&amp;",","")</f>
+        <v>9.99520674372535,</v>
       </c>
       <c r="C45" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D52&amp;"},","}}")</f>
@@ -14248,8 +14247,8 @@
         <v>{2.15,</v>
       </c>
       <c r="B46" t="str">
-        <f>IF(Sheet1!F53=0,","&amp;Sheet1!C53&amp;",","")</f>
-        <v>,9.97613512664259,</v>
+        <f>IF(Sheet1!F53=0,Sheet1!C53&amp;",","")</f>
+        <v>9.97613512664259,</v>
       </c>
       <c r="C46" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D53&amp;"},","}}")</f>
@@ -14262,8 +14261,8 @@
         <v>{2.2,</v>
       </c>
       <c r="B47" t="str">
-        <f>IF(Sheet1!F54=0,","&amp;Sheet1!C54&amp;",","")</f>
-        <v>,9.9425555677179,</v>
+        <f>IF(Sheet1!F54=0,Sheet1!C54&amp;",","")</f>
+        <v>9.9425555677179,</v>
       </c>
       <c r="C47" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D54&amp;"},","}}")</f>
@@ -14276,8 +14275,8 @@
         <v>{2.25,</v>
       </c>
       <c r="B48" t="str">
-        <f>IF(Sheet1!F55=0,","&amp;Sheet1!C55&amp;",","")</f>
-        <v>,9.89451690052078,</v>
+        <f>IF(Sheet1!F55=0,Sheet1!C55&amp;",","")</f>
+        <v>9.89451690052078,</v>
       </c>
       <c r="C48" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D55&amp;"},","}}")</f>
@@ -14290,8 +14289,8 @@
         <v>{2.3,</v>
       </c>
       <c r="B49" t="str">
-        <f>IF(Sheet1!F56=0,","&amp;Sheet1!C56&amp;",","")</f>
-        <v>,9.83208898599245,</v>
+        <f>IF(Sheet1!F56=0,Sheet1!C56&amp;",","")</f>
+        <v>9.83208898599245,</v>
       </c>
       <c r="C49" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D56&amp;"},","}}")</f>
@@ -14304,8 +14303,8 @@
         <v>{2.35,</v>
       </c>
       <c r="B50" t="str">
-        <f>IF(Sheet1!F57=0,","&amp;Sheet1!C57&amp;",","")</f>
-        <v>,9.75536261084961,</v>
+        <f>IF(Sheet1!F57=0,Sheet1!C57&amp;",","")</f>
+        <v>9.75536261084961,</v>
       </c>
       <c r="C50" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D57&amp;"},","}}")</f>
@@ -14318,8 +14317,8 @@
         <v>{2.4,</v>
       </c>
       <c r="B51" t="str">
-        <f>IF(Sheet1!F58=0,","&amp;Sheet1!C58&amp;",","")</f>
-        <v>,9.66444935555644,</v>
+        <f>IF(Sheet1!F58=0,Sheet1!C58&amp;",","")</f>
+        <v>9.66444935555644,</v>
       </c>
       <c r="C51" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D58&amp;"},","}}")</f>
@@ -14332,8 +14331,8 @@
         <v>{2.45,</v>
       </c>
       <c r="B52" t="str">
-        <f>IF(Sheet1!F59=0,","&amp;Sheet1!C59&amp;",","")</f>
-        <v>,9.55948143205713,</v>
+        <f>IF(Sheet1!F59=0,Sheet1!C59&amp;",","")</f>
+        <v>9.55948143205713,</v>
       </c>
       <c r="C52" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D59&amp;"},","}}")</f>
@@ -14346,8 +14345,8 @@
         <v>{2.5,</v>
       </c>
       <c r="B53" t="str">
-        <f>IF(Sheet1!F60=0,","&amp;Sheet1!C60&amp;",","")</f>
-        <v>,9.44061149150466,</v>
+        <f>IF(Sheet1!F60=0,Sheet1!C60&amp;",","")</f>
+        <v>9.44061149150466,</v>
       </c>
       <c r="C53" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D60&amp;"},","}}")</f>
@@ -14360,8 +14359,8 @@
         <v>{2.55,</v>
       </c>
       <c r="B54" t="str">
-        <f>IF(Sheet1!F61=0,","&amp;Sheet1!C61&amp;",","")</f>
-        <v>,9.30801240226561,</v>
+        <f>IF(Sheet1!F61=0,Sheet1!C61&amp;",","")</f>
+        <v>9.30801240226561,</v>
       </c>
       <c r="C54" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D61&amp;"},","}}")</f>
@@ -14374,8 +14373,8 @@
         <v>{2.6,</v>
       </c>
       <c r="B55" t="str">
-        <f>IF(Sheet1!F62=0,","&amp;Sheet1!C62&amp;",","")</f>
-        <v>,9.16187699852383,</v>
+        <f>IF(Sheet1!F62=0,Sheet1!C62&amp;",","")</f>
+        <v>9.16187699852383,</v>
       </c>
       <c r="C55" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D62&amp;"},","}}")</f>
@@ -14388,8 +14387,8 @@
         <v>{2.65,</v>
       </c>
       <c r="B56" t="str">
-        <f>IF(Sheet1!F63=0,","&amp;Sheet1!C63&amp;",","")</f>
-        <v>,9.00241779984844,</v>
+        <f>IF(Sheet1!F63=0,Sheet1!C63&amp;",","")</f>
+        <v>9.00241779984844,</v>
       </c>
       <c r="C56" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D63&amp;"},","}}")</f>
@@ -14402,8 +14401,8 @@
         <v>{2.7,</v>
       </c>
       <c r="B57" t="str">
-        <f>IF(Sheet1!F64=0,","&amp;Sheet1!C64&amp;",","")</f>
-        <v>,8.82986670213409,</v>
+        <f>IF(Sheet1!F64=0,Sheet1!C64&amp;",","")</f>
+        <v>8.82986670213409,</v>
       </c>
       <c r="C57" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D64&amp;"},","}}")</f>
@@ -14416,8 +14415,8 @@
         <v>{2.75,</v>
       </c>
       <c r="B58" t="str">
-        <f>IF(Sheet1!F65=0,","&amp;Sheet1!C65&amp;",","")</f>
-        <v>,8.64447464036299,</v>
+        <f>IF(Sheet1!F65=0,Sheet1!C65&amp;",","")</f>
+        <v>8.64447464036299,</v>
       </c>
       <c r="C58" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D65&amp;"},","}}")</f>
@@ -14430,8 +14429,8 @@
         <v>{2.8,</v>
       </c>
       <c r="B59" t="str">
-        <f>IF(Sheet1!F66=0,","&amp;Sheet1!C66&amp;",","")</f>
-        <v>,8.44651122367896,</v>
+        <f>IF(Sheet1!F66=0,Sheet1!C66&amp;",","")</f>
+        <v>8.44651122367896,</v>
       </c>
       <c r="C59" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D66&amp;"},","}}")</f>
@@ -14444,8 +14443,8 @@
         <v>{2.85,</v>
       </c>
       <c r="B60" t="str">
-        <f>IF(Sheet1!F67=0,","&amp;Sheet1!C67&amp;",","")</f>
-        <v>,8.23626434330436,</v>
+        <f>IF(Sheet1!F67=0,Sheet1!C67&amp;",","")</f>
+        <v>8.23626434330436,</v>
       </c>
       <c r="C60" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D67&amp;"},","}}")</f>
@@ -14458,8 +14457,8 @@
         <v>{2.9,</v>
       </c>
       <c r="B61" t="str">
-        <f>IF(Sheet1!F68=0,","&amp;Sheet1!C68&amp;",","")</f>
-        <v>,8.01403975387004,</v>
+        <f>IF(Sheet1!F68=0,Sheet1!C68&amp;",","")</f>
+        <v>8.01403975387004,</v>
       </c>
       <c r="C61" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D68&amp;"},","}}")</f>
@@ -14472,8 +14471,8 @@
         <v>{2.95,</v>
       </c>
       <c r="B62" t="str">
-        <f>IF(Sheet1!F69=0,","&amp;Sheet1!C69&amp;",","")</f>
-        <v>,7.78016062876715,</v>
+        <f>IF(Sheet1!F69=0,Sheet1!C69&amp;",","")</f>
+        <v>7.78016062876715,</v>
       </c>
       <c r="C62" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D69&amp;"},","}}")</f>
@@ -14486,8 +14485,8 @@
         <v>{3,</v>
       </c>
       <c r="B63" t="str">
-        <f>IF(Sheet1!F70=0,","&amp;Sheet1!C70&amp;",","")</f>
-        <v>,7.53496709016743,</v>
+        <f>IF(Sheet1!F70=0,Sheet1!C70&amp;",","")</f>
+        <v>7.53496709016743,</v>
       </c>
       <c r="C63" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D70&amp;"},","}}")</f>
@@ -14500,8 +14499,8 @@
         <v>{3.05,</v>
       </c>
       <c r="B64" t="str">
-        <f>IF(Sheet1!F71=0,","&amp;Sheet1!C71&amp;",","")</f>
-        <v>,7.27881571439557,</v>
+        <f>IF(Sheet1!F71=0,Sheet1!C71&amp;",","")</f>
+        <v>7.27881571439557,</v>
       </c>
       <c r="C64" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D71&amp;"},","}}")</f>
@@ -14514,8 +14513,8 @@
         <v>{3.1,</v>
       </c>
       <c r="B65" t="str">
-        <f>IF(Sheet1!F72=0,","&amp;Sheet1!C72&amp;",","")</f>
-        <v>,7.01207901337281,</v>
+        <f>IF(Sheet1!F72=0,Sheet1!C72&amp;",","")</f>
+        <v>7.01207901337281,</v>
       </c>
       <c r="C65" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D72&amp;"},","}}")</f>
@@ -14528,8 +14527,8 @@
         <v>{3.15,</v>
       </c>
       <c r="B66" t="str">
-        <f>IF(Sheet1!F73=0,","&amp;Sheet1!C73&amp;",","")</f>
-        <v>,6.73514489288593,</v>
+        <f>IF(Sheet1!F73=0,Sheet1!C73&amp;",","")</f>
+        <v>6.73514489288593,</v>
       </c>
       <c r="C66" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D73&amp;"},","}}")</f>
@@ -14542,8 +14541,8 @@
         <v>{3.2,</v>
       </c>
       <c r="B67" t="str">
-        <f>IF(Sheet1!F74=0,","&amp;Sheet1!C74&amp;",","")</f>
-        <v>,6.44841608846961,</v>
+        <f>IF(Sheet1!F74=0,Sheet1!C74&amp;",","")</f>
+        <v>6.44841608846961,</v>
       </c>
       <c r="C67" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D74&amp;"},","}}")</f>
@@ -14556,8 +14555,8 @@
         <v>{3.25,</v>
       </c>
       <c r="B68" t="str">
-        <f>IF(Sheet1!F75=0,","&amp;Sheet1!C75&amp;",","")</f>
-        <v>,6.15230957972225,</v>
+        <f>IF(Sheet1!F75=0,Sheet1!C75&amp;",","")</f>
+        <v>6.15230957972225,</v>
       </c>
       <c r="C68" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D75&amp;"},","}}")</f>
@@ -14570,8 +14569,8 @@
         <v>{3.3,</v>
       </c>
       <c r="B69" t="str">
-        <f>IF(Sheet1!F76=0,","&amp;Sheet1!C76&amp;",","")</f>
-        <v>,5.84725598390731,</v>
+        <f>IF(Sheet1!F76=0,Sheet1!C76&amp;",","")</f>
+        <v>5.84725598390731,</v>
       </c>
       <c r="C69" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D76&amp;"},","}}")</f>
@@ -14584,8 +14583,8 @@
         <v>{3.35,</v>
       </c>
       <c r="B70" t="str">
-        <f>IF(Sheet1!F77=0,","&amp;Sheet1!C77&amp;",","")</f>
-        <v>,5.53369892972171,</v>
+        <f>IF(Sheet1!F77=0,Sheet1!C77&amp;",","")</f>
+        <v>5.53369892972171,</v>
       </c>
       <c r="C70" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D77&amp;"},","}}")</f>
@@ -14598,8 +14597,8 @@
         <v>{3.4,</v>
       </c>
       <c r="B71" t="str">
-        <f>IF(Sheet1!F78=0,","&amp;Sheet1!C78&amp;",","")</f>
-        <v>,5.21209441214233,</v>
+        <f>IF(Sheet1!F78=0,Sheet1!C78&amp;",","")</f>
+        <v>5.21209441214233,</v>
       </c>
       <c r="C71" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D78&amp;"},","}}")</f>
@@ -14612,8 +14611,8 @@
         <v>{3.45,</v>
       </c>
       <c r="B72" t="str">
-        <f>IF(Sheet1!F79=0,","&amp;Sheet1!C79&amp;",","")</f>
-        <v>,4.88291012928851,</v>
+        <f>IF(Sheet1!F79=0,Sheet1!C79&amp;",","")</f>
+        <v>4.88291012928851,</v>
       </c>
       <c r="C72" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D79&amp;"},","}}")</f>
@@ -14626,8 +14625,8 @@
         <v>{3.5,</v>
       </c>
       <c r="B73" t="str">
-        <f>IF(Sheet1!F80=0,","&amp;Sheet1!C80&amp;",","")</f>
-        <v>,4.54662480226521,</v>
+        <f>IF(Sheet1!F80=0,Sheet1!C80&amp;",","")</f>
+        <v>4.54662480226521,</v>
       </c>
       <c r="C73" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D80&amp;"},","}}")</f>
@@ -14640,8 +14639,8 @@
         <v>{3.55,</v>
       </c>
       <c r="B74" t="str">
-        <f>IF(Sheet1!F81=0,","&amp;Sheet1!C81&amp;",","")</f>
-        <v>,4.20372747897572,</v>
+        <f>IF(Sheet1!F81=0,Sheet1!C81&amp;",","")</f>
+        <v>4.20372747897572,</v>
       </c>
       <c r="C74" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D81&amp;"},","}}")</f>
@@ -14654,8 +14653,8 @@
         <v>{3.6,</v>
       </c>
       <c r="B75" t="str">
-        <f>IF(Sheet1!F82=0,","&amp;Sheet1!C82&amp;",","")</f>
-        <v>,3.85471682291657,</v>
+        <f>IF(Sheet1!F82=0,Sheet1!C82&amp;",","")</f>
+        <v>3.85471682291657,</v>
       </c>
       <c r="C75" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D82&amp;"},","}}")</f>
@@ -14668,8 +14667,8 @@
         <v>{3.65,</v>
       </c>
       <c r="B76" t="str">
-        <f>IF(Sheet1!F83=0,","&amp;Sheet1!C83&amp;",","")</f>
-        <v>,3.50010038798874,</v>
+        <f>IF(Sheet1!F83=0,Sheet1!C83&amp;",","")</f>
+        <v>3.50010038798874,</v>
       </c>
       <c r="C76" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D83&amp;"},","}}")</f>
@@ -14682,8 +14681,8 @@
         <v>{3.69999999999999,</v>
       </c>
       <c r="B77" t="str">
-        <f>IF(Sheet1!F84=0,","&amp;Sheet1!C84&amp;",","")</f>
-        <v>,3.14039388037994,</v>
+        <f>IF(Sheet1!F84=0,Sheet1!C84&amp;",","")</f>
+        <v>3.14039388037994,</v>
       </c>
       <c r="C77" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D84&amp;"},","}}")</f>
@@ -14696,8 +14695,8 @@
         <v>{3.74999999999999,</v>
       </c>
       <c r="B78" t="str">
-        <f>IF(Sheet1!F85=0,","&amp;Sheet1!C85&amp;",","")</f>
-        <v>,2.77612040859123,</v>
+        <f>IF(Sheet1!F85=0,Sheet1!C85&amp;",","")</f>
+        <v>2.77612040859123,</v>
       </c>
       <c r="C78" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D85&amp;"},","}}")</f>
@@ -14710,8 +14709,8 @@
         <v>{3.79999999999999,</v>
       </c>
       <c r="B79" t="str">
-        <f>IF(Sheet1!F86=0,","&amp;Sheet1!C86&amp;",","")</f>
-        <v>,2.40780972269879,</v>
+        <f>IF(Sheet1!F86=0,Sheet1!C86&amp;",","")</f>
+        <v>2.40780972269879,</v>
       </c>
       <c r="C79" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D86&amp;"},","}}")</f>
@@ -14724,8 +14723,8 @@
         <v>{3.84999999999999,</v>
       </c>
       <c r="B80" t="str">
-        <f>IF(Sheet1!F87=0,","&amp;Sheet1!C87&amp;",","")</f>
-        <v>,2.03599744395702,</v>
+        <f>IF(Sheet1!F87=0,Sheet1!C87&amp;",","")</f>
+        <v>2.03599744395702,</v>
       </c>
       <c r="C80" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D87&amp;"},","}}")</f>
@@ -14738,8 +14737,8 @@
         <v>{3.89999999999999,</v>
       </c>
       <c r="B81" t="str">
-        <f>IF(Sheet1!F88=0,","&amp;Sheet1!C88&amp;",","")</f>
-        <v>,1.66122428586346,</v>
+        <f>IF(Sheet1!F88=0,Sheet1!C88&amp;",","")</f>
+        <v>1.66122428586346,</v>
       </c>
       <c r="C81" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D88&amp;"},","}}")</f>
@@ -14752,8 +14751,8 @@
         <v>{3.94999999999999,</v>
       </c>
       <c r="B82" t="str">
-        <f>IF(Sheet1!F89=0,","&amp;Sheet1!C89&amp;",","")</f>
-        <v>,1.28403526781814,</v>
+        <f>IF(Sheet1!F89=0,Sheet1!C89&amp;",","")</f>
+        <v>1.28403526781814,</v>
       </c>
       <c r="C82" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D89&amp;"},","}}")</f>
@@ -14766,8 +14765,8 @@
         <v>{3.99999999999999,</v>
       </c>
       <c r="B83" t="str">
-        <f>IF(Sheet1!F90=0,","&amp;Sheet1!C90&amp;",","")</f>
-        <v>,0.904978922521143,</v>
+        <f>IF(Sheet1!F90=0,Sheet1!C90&amp;",","")</f>
+        <v>0.904978922521143,</v>
       </c>
       <c r="C83" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D90&amp;"},","}}")</f>
@@ -14780,8 +14779,8 @@
         <v>{4.04999999999999,</v>
       </c>
       <c r="B84" t="str">
-        <f>IF(Sheet1!F91=0,","&amp;Sheet1!C91&amp;",","")</f>
-        <v>,0.524606498260752,</v>
+        <f>IF(Sheet1!F91=0,Sheet1!C91&amp;",","")</f>
+        <v>0.524606498260752,</v>
       </c>
       <c r="C84" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D91&amp;"},","}}")</f>
@@ -14794,8 +14793,8 @@
         <v>{4.09999999999999,</v>
       </c>
       <c r="B85" t="str">
-        <f>IF(Sheet1!F92=0,","&amp;Sheet1!C92&amp;",","")</f>
-        <v>,0.143471157252538,</v>
+        <f>IF(Sheet1!F92=0,Sheet1!C92&amp;",","")</f>
+        <v>0.143471157252538,</v>
       </c>
       <c r="C85" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D92&amp;"},","}}")</f>
@@ -14808,8 +14807,8 @@
         <v>{4.14999999999999,</v>
       </c>
       <c r="B86" t="str">
-        <f>IF(Sheet1!F93=0,","&amp;Sheet1!C93&amp;",","")</f>
-        <v>,-0.237872828804985,</v>
+        <f>IF(Sheet1!F93=0,Sheet1!C93&amp;",","")</f>
+        <v>-0.237872828804985,</v>
       </c>
       <c r="C86" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D93&amp;"},","}}")</f>
@@ -14822,8 +14821,8 @@
         <v>{4.19999999999999,</v>
       </c>
       <c r="B87" t="str">
-        <f>IF(Sheet1!F94=0,","&amp;Sheet1!C94&amp;",","")</f>
-        <v>,-0.618870884788159,</v>
+        <f>IF(Sheet1!F94=0,Sheet1!C94&amp;",","")</f>
+        <v>-0.618870884788159,</v>
       </c>
       <c r="C87" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D94&amp;"},","}}")</f>
@@ -14836,8 +14835,8 @@
         <v>{4.24999999999999,</v>
       </c>
       <c r="B88" t="str">
-        <f>IF(Sheet1!F95=0,","&amp;Sheet1!C95&amp;",","")</f>
-        <v>,-0.998968938647246,</v>
+        <f>IF(Sheet1!F95=0,Sheet1!C95&amp;",","")</f>
+        <v>-0.998968938647246,</v>
       </c>
       <c r="C88" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D95&amp;"},","}}")</f>
@@ -14850,8 +14849,8 @@
         <v>{4.29999999999999,</v>
       </c>
       <c r="B89" t="str">
-        <f>IF(Sheet1!F96=0,","&amp;Sheet1!C96&amp;",","")</f>
-        <v>,-1.37761422717389,</v>
+        <f>IF(Sheet1!F96=0,Sheet1!C96&amp;",","")</f>
+        <v>-1.37761422717389,</v>
       </c>
       <c r="C89" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D96&amp;"},","}}")</f>
@@ -14864,8 +14863,8 @@
         <v>{4.34999999999999,</v>
       </c>
       <c r="B90" t="str">
-        <f>IF(Sheet1!F97=0,","&amp;Sheet1!C97&amp;",","")</f>
-        <v>,-1.75425609986516,</v>
+        <f>IF(Sheet1!F97=0,Sheet1!C97&amp;",","")</f>
+        <v>-1.75425609986516,</v>
       </c>
       <c r="C90" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D97&amp;"},","}}")</f>
@@ -14878,8 +14877,8 @@
         <v>{4.39999999999999,</v>
       </c>
       <c r="B91" t="str">
-        <f>IF(Sheet1!F98=0,","&amp;Sheet1!C98&amp;",","")</f>
-        <v>,-2.12834681971522,</v>
+        <f>IF(Sheet1!F98=0,Sheet1!C98&amp;",","")</f>
+        <v>-2.12834681971522,</v>
       </c>
       <c r="C91" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D98&amp;"},","}}")</f>
@@ -14892,8 +14891,8 @@
         <v>{4.44999999999999,</v>
       </c>
       <c r="B92" t="str">
-        <f>IF(Sheet1!F99=0,","&amp;Sheet1!C99&amp;",","")</f>
-        <v>,-2.49934235976991,</v>
+        <f>IF(Sheet1!F99=0,Sheet1!C99&amp;",","")</f>
+        <v>-2.49934235976991,</v>
       </c>
       <c r="C92" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D99&amp;"},","}}")</f>
@@ -14906,8 +14905,8 @@
         <v>{4.49999999999999,</v>
       </c>
       <c r="B93" t="str">
-        <f>IF(Sheet1!F100=0,","&amp;Sheet1!C100&amp;",","")</f>
-        <v>,-2.86670319428601,</v>
+        <f>IF(Sheet1!F100=0,Sheet1!C100&amp;",","")</f>
+        <v>-2.86670319428601,</v>
       </c>
       <c r="C93" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D100&amp;"},","}}")</f>
@@ -14920,8 +14919,8 @@
         <v>{4.54999999999999,</v>
       </c>
       <c r="B94" t="str">
-        <f>IF(Sheet1!F101=0,","&amp;Sheet1!C101&amp;",","")</f>
-        <v>,-3.22989508334448,</v>
+        <f>IF(Sheet1!F101=0,Sheet1!C101&amp;",","")</f>
+        <v>-3.22989508334448,</v>
       </c>
       <c r="C94" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D101&amp;"},","}}")</f>
@@ -14934,8 +14933,8 @@
         <v>{4.59999999999999,</v>
       </c>
       <c r="B95" t="str">
-        <f>IF(Sheet1!F102=0,","&amp;Sheet1!C102&amp;",","")</f>
-        <v>,-3.58838984977683,</v>
+        <f>IF(Sheet1!F102=0,Sheet1!C102&amp;",","")</f>
+        <v>-3.58838984977683,</v>
       </c>
       <c r="C95" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D102&amp;"},","}}")</f>
@@ -14948,8 +14947,8 @@
         <v>{4.64999999999999,</v>
       </c>
       <c r="B96" t="str">
-        <f>IF(Sheet1!F103=0,","&amp;Sheet1!C103&amp;",","")</f>
-        <v>,-3.94166614727448,</v>
+        <f>IF(Sheet1!F103=0,Sheet1!C103&amp;",","")</f>
+        <v>-3.94166614727448,</v>
       </c>
       <c r="C96" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D103&amp;"},","}}")</f>
@@ -14962,8 +14961,8 @@
         <v>{4.69999999999999,</v>
       </c>
       <c r="B97" t="str">
-        <f>IF(Sheet1!F104=0,","&amp;Sheet1!C104&amp;",","")</f>
-        <v>,-4.28921021856439,</v>
+        <f>IF(Sheet1!F104=0,Sheet1!C104&amp;",","")</f>
+        <v>-4.28921021856439,</v>
       </c>
       <c r="C97" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D104&amp;"},","}}")</f>
@@ -14976,8 +14975,8 @@
         <v>{4.74999999999999,</v>
       </c>
       <c r="B98" t="str">
-        <f>IF(Sheet1!F105=0,","&amp;Sheet1!C105&amp;",","")</f>
-        <v>,-4.63051664254812,</v>
+        <f>IF(Sheet1!F105=0,Sheet1!C105&amp;",","")</f>
+        <v>-4.63051664254812,</v>
       </c>
       <c r="C98" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D105&amp;"},","}}")</f>
@@ -14990,8 +14989,8 @@
         <v>{4.79999999999999,</v>
       </c>
       <c r="B99" t="str">
-        <f>IF(Sheet1!F106=0,","&amp;Sheet1!C106&amp;",","")</f>
-        <v>,-4.96508906931796,</v>
+        <f>IF(Sheet1!F106=0,Sheet1!C106&amp;",","")</f>
+        <v>-4.96508906931796,</v>
       </c>
       <c r="C99" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D106&amp;"},","}}")</f>
@@ -15004,8 +15003,8 @@
         <v>{4.84999999999999,</v>
       </c>
       <c r="B100" t="str">
-        <f>IF(Sheet1!F107=0,","&amp;Sheet1!C107&amp;",","")</f>
-        <v>,-5.29244094198111,</v>
+        <f>IF(Sheet1!F107=0,Sheet1!C107&amp;",","")</f>
+        <v>-5.29244094198111,</v>
       </c>
       <c r="C100" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D107&amp;"},","}}")</f>
@@ -15018,8 +15017,8 @@
         <v>{4.89999999999999,</v>
       </c>
       <c r="B101" t="str">
-        <f>IF(Sheet1!F108=0,","&amp;Sheet1!C108&amp;",","")</f>
-        <v>,-5.6120962042422,</v>
+        <f>IF(Sheet1!F108=0,Sheet1!C108&amp;",","")</f>
+        <v>-5.6120962042422,</v>
       </c>
       <c r="C101" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D108&amp;"},","}}")</f>
@@ -15032,8 +15031,8 @@
         <v>{4.94999999999999,</v>
       </c>
       <c r="B102" t="str">
-        <f>IF(Sheet1!F109=0,","&amp;Sheet1!C109&amp;",","")</f>
-        <v>,-5.9235899927152,</v>
+        <f>IF(Sheet1!F109=0,Sheet1!C109&amp;",","")</f>
+        <v>-5.9235899927152,</v>
       </c>
       <c r="C102" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D109&amp;"},","}}")</f>
@@ -15046,8 +15045,8 @@
         <v>{4.99999999999999,</v>
       </c>
       <c r="B103" t="str">
-        <f>IF(Sheet1!F110=0,","&amp;Sheet1!C110&amp;",","")</f>
-        <v>,-6.2264693129579,</v>
+        <f>IF(Sheet1!F110=0,Sheet1!C110&amp;",","")</f>
+        <v>-6.2264693129579,</v>
       </c>
       <c r="C103" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D110&amp;"},","}}")</f>
@@ -15060,8 +15059,8 @@
         <v>{5.04999999999999,</v>
       </c>
       <c r="B104" t="str">
-        <f>IF(Sheet1!F111=0,","&amp;Sheet1!C111&amp;",","")</f>
-        <v>,-6.52029369824571,</v>
+        <f>IF(Sheet1!F111=0,Sheet1!C111&amp;",","")</f>
+        <v>-6.52029369824571,</v>
       </c>
       <c r="C104" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D111&amp;"},","}}")</f>
@@ -15074,8 +15073,8 @@
         <v>{5.09999999999999,</v>
       </c>
       <c r="B105" t="str">
-        <f>IF(Sheet1!F112=0,","&amp;Sheet1!C112&amp;",","")</f>
-        <v>,-6.80463585012694,</v>
+        <f>IF(Sheet1!F112=0,Sheet1!C112&amp;",","")</f>
+        <v>-6.80463585012694,</v>
       </c>
       <c r="C105" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D112&amp;"},","}}")</f>
@@ -15088,8 +15087,8 @@
         <v>{5.14999999999999,</v>
       </c>
       <c r="B106" t="str">
-        <f>IF(Sheet1!F113=0,","&amp;Sheet1!C113&amp;",","")</f>
-        <v>,-7.07908225982786,</v>
+        <f>IF(Sheet1!F113=0,Sheet1!C113&amp;",","")</f>
+        <v>-7.07908225982786,</v>
       </c>
       <c r="C106" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D113&amp;"},","}}")</f>
@@ -15102,8 +15101,8 @@
         <v>{5.19999999999999,</v>
       </c>
       <c r="B107" t="str">
-        <f>IF(Sheet1!F114=0,","&amp;Sheet1!C114&amp;",","")</f>
-        <v>,-7.34323380960397,</v>
+        <f>IF(Sheet1!F114=0,Sheet1!C114&amp;",","")</f>
+        <v>-7.34323380960397,</v>
       </c>
       <c r="C107" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D114&amp;"},","}}")</f>
@@ -15116,8 +15115,8 @@
         <v>{5.24999999999999,</v>
       </c>
       <c r="B108" t="str">
-        <f>IF(Sheet1!F115=0,","&amp;Sheet1!C115&amp;",","")</f>
-        <v>,-7.59670635316285,</v>
+        <f>IF(Sheet1!F115=0,Sheet1!C115&amp;",","")</f>
+        <v>-7.59670635316285,</v>
       </c>
       <c r="C108" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D115&amp;"},","}}")</f>
@@ -15130,8 +15129,8 @@
         <v>{5.29999999999999,</v>
       </c>
       <c r="B109" t="str">
-        <f>IF(Sheet1!F116=0,","&amp;Sheet1!C116&amp;",","")</f>
-        <v>,-7.83913127431457,</v>
+        <f>IF(Sheet1!F116=0,Sheet1!C116&amp;",","")</f>
+        <v>-7.83913127431457,</v>
       </c>
       <c r="C109" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D116&amp;"},","}}")</f>
@@ -15144,8 +15143,8 @@
         <v>{5.34999999999999,</v>
       </c>
       <c r="B110" t="str">
-        <f>IF(Sheet1!F117=0,","&amp;Sheet1!C117&amp;",","")</f>
-        <v>,-8.07015602303727,</v>
+        <f>IF(Sheet1!F117=0,Sheet1!C117&amp;",","")</f>
+        <v>-8.07015602303727,</v>
       </c>
       <c r="C110" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D117&amp;"},","}}")</f>
@@ -15158,8 +15157,8 @@
         <v>{5.39999999999999,</v>
       </c>
       <c r="B111" t="str">
-        <f>IF(Sheet1!F118=0,","&amp;Sheet1!C118&amp;",","")</f>
-        <v>,-8.28944462817819,</v>
+        <f>IF(Sheet1!F118=0,Sheet1!C118&amp;",","")</f>
+        <v>-8.28944462817819,</v>
       </c>
       <c r="C111" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D118&amp;"},","}}")</f>
@@ -15172,8 +15171,8 @@
         <v>{5.44999999999999,</v>
       </c>
       <c r="B112" t="str">
-        <f>IF(Sheet1!F119=0,","&amp;Sheet1!C119&amp;",","")</f>
-        <v>,-8.49667818604471,</v>
+        <f>IF(Sheet1!F119=0,Sheet1!C119&amp;",","")</f>
+        <v>-8.49667818604471,</v>
       </c>
       <c r="C112" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D119&amp;"},","}}")</f>
@@ -15186,8 +15185,8 @@
         <v>{5.49999999999999,</v>
       </c>
       <c r="B113" t="str">
-        <f>IF(Sheet1!F120=0,","&amp;Sheet1!C120&amp;",","")</f>
-        <v>,-8.69155532417474,</v>
+        <f>IF(Sheet1!F120=0,Sheet1!C120&amp;",","")</f>
+        <v>-8.69155532417474,</v>
       </c>
       <c r="C113" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D120&amp;"},","}}")</f>
@@ -15200,8 +15199,8 @@
         <v>{5.54999999999999,</v>
       </c>
       <c r="B114" t="str">
-        <f>IF(Sheet1!F121=0,","&amp;Sheet1!C121&amp;",","")</f>
-        <v>,-8.8737926396121,</v>
+        <f>IF(Sheet1!F121=0,Sheet1!C121&amp;",","")</f>
+        <v>-8.8737926396121,</v>
       </c>
       <c r="C114" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D121&amp;"},","}}")</f>
@@ -15214,8 +15213,8 @@
         <v>{5.59999999999999,</v>
       </c>
       <c r="B115" t="str">
-        <f>IF(Sheet1!F122=0,","&amp;Sheet1!C122&amp;",","")</f>
-        <v>,-9.04312511104939,</v>
+        <f>IF(Sheet1!F122=0,Sheet1!C122&amp;",","")</f>
+        <v>-9.04312511104939,</v>
       </c>
       <c r="C115" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D122&amp;"},","}}")</f>
@@ -15228,8 +15227,8 @@
         <v>{5.64999999999999,</v>
       </c>
       <c r="B116" t="str">
-        <f>IF(Sheet1!F123=0,","&amp;Sheet1!C123&amp;",","")</f>
-        <v>,-9.19930648423923,</v>
+        <f>IF(Sheet1!F123=0,Sheet1!C123&amp;",","")</f>
+        <v>-9.19930648423923,</v>
       </c>
       <c r="C116" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D123&amp;"},","}}")</f>
@@ -15242,8 +15241,8 @@
         <v>{5.69999999999999,</v>
       </c>
       <c r="B117" t="str">
-        <f>IF(Sheet1!F124=0,","&amp;Sheet1!C124&amp;",","")</f>
-        <v>,-9.34210963011307,</v>
+        <f>IF(Sheet1!F124=0,Sheet1!C124&amp;",","")</f>
+        <v>-9.34210963011307,</v>
       </c>
       <c r="C117" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D124&amp;"},","}}")</f>
@@ -15256,8 +15255,8 @@
         <v>{5.74999999999999,</v>
       </c>
       <c r="B118" t="str">
-        <f>IF(Sheet1!F125=0,","&amp;Sheet1!C125&amp;",","")</f>
-        <v>,-9.471326875087,</v>
+        <f>IF(Sheet1!F125=0,Sheet1!C125&amp;",","")</f>
+        <v>-9.471326875087,</v>
       </c>
       <c r="C118" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D125&amp;"},","}}")</f>
@@ -15270,8 +15269,8 @@
         <v>{5.79999999999999,</v>
       </c>
       <c r="B119" t="str">
-        <f>IF(Sheet1!F126=0,","&amp;Sheet1!C126&amp;",","")</f>
-        <v>,-9.58677030307418,</v>
+        <f>IF(Sheet1!F126=0,Sheet1!C126&amp;",","")</f>
+        <v>-9.58677030307418,</v>
       </c>
       <c r="C119" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D126&amp;"},","}}")</f>
@@ -15284,8 +15283,8 @@
         <v>{5.84999999999999,</v>
       </c>
       <c r="B120" t="str">
-        <f>IF(Sheet1!F127=0,","&amp;Sheet1!C127&amp;",","")</f>
-        <v>,-9.68827202876448,</v>
+        <f>IF(Sheet1!F127=0,Sheet1!C127&amp;",","")</f>
+        <v>-9.68827202876448,</v>
       </c>
       <c r="C120" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D127&amp;"},","}}")</f>
@@ -15298,8 +15297,8 @@
         <v>{5.89999999999999,</v>
       </c>
       <c r="B121" t="str">
-        <f>IF(Sheet1!F128=0,","&amp;Sheet1!C128&amp;",","")</f>
-        <v>,-9.7756844417743,</v>
+        <f>IF(Sheet1!F128=0,Sheet1!C128&amp;",","")</f>
+        <v>-9.7756844417743,</v>
       </c>
       <c r="C121" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D128&amp;"},","}}")</f>
@@ -15312,8 +15311,8 @@
         <v>{5.94999999999999,</v>
       </c>
       <c r="B122" t="str">
-        <f>IF(Sheet1!F129=0,","&amp;Sheet1!C129&amp;",","")</f>
-        <v>,-9.84888042131105,</v>
+        <f>IF(Sheet1!F129=0,Sheet1!C129&amp;",","")</f>
+        <v>-9.84888042131105,</v>
       </c>
       <c r="C122" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D129&amp;"},","}}")</f>
@@ -15326,8 +15325,8 @@
         <v>{5.99999999999999,</v>
       </c>
       <c r="B123" t="str">
-        <f>IF(Sheet1!F130=0,","&amp;Sheet1!C130&amp;",","")</f>
-        <v>,-9.90775352104049,</v>
+        <f>IF(Sheet1!F130=0,Sheet1!C130&amp;",","")</f>
+        <v>-9.90775352104049,</v>
       </c>
       <c r="C123" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D130&amp;"},","}}")</f>
@@ -15340,8 +15339,8 @@
         <v>{6.04999999999999,</v>
       </c>
       <c r="B124" t="str">
-        <f>IF(Sheet1!F131=0,","&amp;Sheet1!C131&amp;",","")</f>
-        <v>,-9.95221812388784,</v>
+        <f>IF(Sheet1!F131=0,Sheet1!C131&amp;",","")</f>
+        <v>-9.95221812388784,</v>
       </c>
       <c r="C124" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D131&amp;"},","}}")</f>
@@ -15354,8 +15353,8 @@
         <v>{6.09999999999999,</v>
       </c>
       <c r="B125" t="str">
-        <f>IF(Sheet1!F132=0,","&amp;Sheet1!C132&amp;",","")</f>
-        <v>,-9.98220956654775,</v>
+        <f>IF(Sheet1!F132=0,Sheet1!C132&amp;",","")</f>
+        <v>-9.98220956654775,</v>
       </c>
       <c r="C125" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D132&amp;"},","}}")</f>
@@ -15368,8 +15367,8 @@
         <v>{6.14999999999999,</v>
       </c>
       <c r="B126" t="str">
-        <f>IF(Sheet1!F133=0,","&amp;Sheet1!C133&amp;",","")</f>
-        <v>,-9.99768423352179,</v>
+        <f>IF(Sheet1!F133=0,Sheet1!C133&amp;",","")</f>
+        <v>-9.99768423352179,</v>
       </c>
       <c r="C126" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D133&amp;"},","}}")</f>
@@ -15382,8 +15381,8 @@
         <v>{6.19999999999999,</v>
       </c>
       <c r="B127" t="str">
-        <f>IF(Sheet1!F134=0,","&amp;Sheet1!C134&amp;",","")</f>
-        <v>,-9.99861962054697,</v>
+        <f>IF(Sheet1!F134=0,Sheet1!C134&amp;",","")</f>
+        <v>-9.99861962054697,</v>
       </c>
       <c r="C127" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D134&amp;"},","}}")</f>
@@ -15396,8 +15395,8 @@
         <v>{6.24999999999999,</v>
       </c>
       <c r="B128" t="str">
-        <f>IF(Sheet1!F135=0,","&amp;Sheet1!C135&amp;",","")</f>
-        <v>,-9.9850143673229,</v>
+        <f>IF(Sheet1!F135=0,Sheet1!C135&amp;",","")</f>
+        <v>-9.9850143673229,</v>
       </c>
       <c r="C128" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D135&amp;"},","}}")</f>
@@ -15410,8 +15409,8 @@
         <v>{6.29999999999999,</v>
       </c>
       <c r="B129" t="str">
-        <f>IF(Sheet1!F136=0,","&amp;Sheet1!C136&amp;",","")</f>
-        <v>,-9.95688825949001,</v>
+        <f>IF(Sheet1!F136=0,Sheet1!C136&amp;",","")</f>
+        <v>-9.95688825949001,</v>
       </c>
       <c r="C129" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D136&amp;"},","}}")</f>
@@ -15424,8 +15423,8 @@
         <v>{6.34999999999999,</v>
       </c>
       <c r="B130" t="str">
-        <f>IF(Sheet1!F137=0,","&amp;Sheet1!C137&amp;",","")</f>
-        <v>,-9.914282199856,</v>
+        <f>IF(Sheet1!F137=0,Sheet1!C137&amp;",","")</f>
+        <v>-9.914282199856,</v>
       </c>
       <c r="C130" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D137&amp;"},","}}")</f>
@@ -15438,8 +15437,8 @@
         <v>{6.39999999999999,</v>
       </c>
       <c r="B131" t="str">
-        <f>IF(Sheet1!F138=0,","&amp;Sheet1!C138&amp;",","")</f>
-        <v>,-9.85725814891233,</v>
+        <f>IF(Sheet1!F138=0,Sheet1!C138&amp;",","")</f>
+        <v>-9.85725814891233,</v>
       </c>
       <c r="C131" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D138&amp;"},","}}")</f>
@@ -15452,8 +15451,8 @@
         <v>{6.44999999999999,</v>
       </c>
       <c r="B132" t="str">
-        <f>IF(Sheet1!F139=0,","&amp;Sheet1!C139&amp;",","")</f>
-        <v>,-9.78589903472725,</v>
+        <f>IF(Sheet1!F139=0,Sheet1!C139&amp;",","")</f>
+        <v>-9.78589903472725,</v>
       </c>
       <c r="C132" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D139&amp;"},","}}")</f>
@@ -15466,8 +15465,8 @@
         <v>{6.49999999999998,</v>
       </c>
       <c r="B133" t="str">
-        <f>IF(Sheet1!F140=0,","&amp;Sheet1!C140&amp;",","")</f>
-        <v>,-9.70030863234644,</v>
+        <f>IF(Sheet1!F140=0,Sheet1!C140&amp;",","")</f>
+        <v>-9.70030863234644,</v>
       </c>
       <c r="C133" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D140&amp;"},","}}")</f>
@@ -15480,8 +15479,8 @@
         <v>{6.54999999999998,</v>
       </c>
       <c r="B134" t="str">
-        <f>IF(Sheet1!F141=0,","&amp;Sheet1!C141&amp;",","")</f>
-        <v>,-9.60061141287662,</v>
+        <f>IF(Sheet1!F141=0,Sheet1!C141&amp;",","")</f>
+        <v>-9.60061141287662,</v>
       </c>
       <c r="C134" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D141&amp;"},","}}")</f>
@@ -15494,8 +15493,8 @@
         <v>{6.59999999999998,</v>
       </c>
       <c r="B135" t="str">
-        <f>IF(Sheet1!F142=0,","&amp;Sheet1!C142&amp;",","")</f>
-        <v>,-9.4869523624716,</v>
+        <f>IF(Sheet1!F142=0,Sheet1!C142&amp;",","")</f>
+        <v>-9.4869523624716,</v>
       </c>
       <c r="C135" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D142&amp;"},","}}")</f>
@@ -15508,8 +15507,8 @@
         <v>{6.64999999999998,</v>
       </c>
       <c r="B136" t="str">
-        <f>IF(Sheet1!F143=0,","&amp;Sheet1!C143&amp;",","")</f>
-        <v>,-9.35949677148401,</v>
+        <f>IF(Sheet1!F143=0,Sheet1!C143&amp;",","")</f>
+        <v>-9.35949677148401,</v>
       </c>
       <c r="C136" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D143&amp;"},","}}")</f>
@@ -15522,8 +15521,8 @@
         <v>{6.69999999999998,</v>
       </c>
       <c r="B137" t="str">
-        <f>IF(Sheet1!F144=0,","&amp;Sheet1!C144&amp;",","")</f>
-        <v>,-9.21842999408939,</v>
+        <f>IF(Sheet1!F144=0,Sheet1!C144&amp;",","")</f>
+        <v>-9.21842999408939,</v>
       </c>
       <c r="C137" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D144&amp;"},","}}")</f>
@@ -15536,8 +15535,8 @@
         <v>{6.74999999999998,</v>
       </c>
       <c r="B138" t="str">
-        <f>IF(Sheet1!F145=0,","&amp;Sheet1!C145&amp;",","")</f>
-        <v>,-9.06395717873215,</v>
+        <f>IF(Sheet1!F145=0,Sheet1!C145&amp;",","")</f>
+        <v>-9.06395717873215,</v>
       </c>
       <c r="C138" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D145&amp;"},","}}")</f>
@@ -15550,8 +15549,8 @@
         <v>{6.79999999999998,</v>
       </c>
       <c r="B139" t="str">
-        <f>IF(Sheet1!F146=0,","&amp;Sheet1!C146&amp;",","")</f>
-        <v>,-8.89630296978536,</v>
+        <f>IF(Sheet1!F146=0,Sheet1!C146&amp;",","")</f>
+        <v>-8.89630296978536,</v>
       </c>
       <c r="C139" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D146&amp;"},","}}")</f>
@@ -15564,8 +15563,8 @@
         <v>{6.84999999999998,</v>
       </c>
       <c r="B140" t="str">
-        <f>IF(Sheet1!F147=0,","&amp;Sheet1!C147&amp;",","")</f>
-        <v>,-8.71571118085841,</v>
+        <f>IF(Sheet1!F147=0,Sheet1!C147&amp;",","")</f>
+        <v>-8.71571118085841,</v>
       </c>
       <c r="C140" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D147&amp;"},","}}")</f>
@@ -15578,8 +15577,8 @@
         <v>{6.89999999999998,</v>
       </c>
       <c r="B141" t="str">
-        <f>IF(Sheet1!F148=0,","&amp;Sheet1!C148&amp;",","")</f>
-        <v>,-8.52244444022745,</v>
+        <f>IF(Sheet1!F148=0,Sheet1!C148&amp;",","")</f>
+        <v>-8.52244444022745,</v>
       </c>
       <c r="C141" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D148&amp;"},","}}")</f>
@@ -15592,8 +15591,8 @@
         <v>{6.94999999999998,</v>
       </c>
       <c r="B142" t="str">
-        <f>IF(Sheet1!F149=0,","&amp;Sheet1!C149&amp;",","")</f>
-        <v>,-8.31678380890433,</v>
+        <f>IF(Sheet1!F149=0,Sheet1!C149&amp;",","")</f>
+        <v>-8.31678380890433,</v>
       </c>
       <c r="C142" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D149&amp;"},","}}")</f>
@@ -15606,8 +15605,8 @@
         <v>{6.99999999999998,</v>
       </c>
       <c r="B143" t="str">
-        <f>IF(Sheet1!F150=0,","&amp;Sheet1!C150&amp;",","")</f>
-        <v>,-8.09902837189947,</v>
+        <f>IF(Sheet1!F150=0,Sheet1!C150&amp;",","")</f>
+        <v>-8.09902837189947,</v>
       </c>
       <c r="C143" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D150&amp;"},","}}")</f>
@@ -15620,8 +15619,8 @@
         <v>{7.04999999999998,</v>
       </c>
       <c r="B144" t="str">
-        <f>IF(Sheet1!F151=0,","&amp;Sheet1!C151&amp;",","")</f>
-        <v>,-7.8694948032731,</v>
+        <f>IF(Sheet1!F151=0,Sheet1!C151&amp;",","")</f>
+        <v>-7.8694948032731,</v>
       </c>
       <c r="C144" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D151&amp;"},","}}")</f>
@@ -15634,8 +15633,8 @@
         <v>{7.09999999999998,</v>
       </c>
       <c r="B145" t="str">
-        <f>IF(Sheet1!F152=0,","&amp;Sheet1!C152&amp;",","")</f>
-        <v>,-7.62851690560728,</v>
+        <f>IF(Sheet1!F152=0,Sheet1!C152&amp;",","")</f>
+        <v>-7.62851690560728,</v>
       </c>
       <c r="C145" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D152&amp;"},","}}")</f>
@@ -15648,8 +15647,8 @@
         <v>{7.14999999999998,</v>
       </c>
       <c r="B146" t="str">
-        <f>IF(Sheet1!F153=0,","&amp;Sheet1!C153&amp;",","")</f>
-        <v>,-7.37644512456862,</v>
+        <f>IF(Sheet1!F153=0,Sheet1!C153&amp;",","")</f>
+        <v>-7.37644512456862,</v>
       </c>
       <c r="C146" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D153&amp;"},","}}")</f>
@@ -15662,8 +15661,8 @@
         <v>{7.19999999999998,</v>
       </c>
       <c r="B147" t="str">
-        <f>IF(Sheet1!F154=0,","&amp;Sheet1!C154&amp;",","")</f>
-        <v>,-7.11364603926745,</v>
+        <f>IF(Sheet1!F154=0,Sheet1!C154&amp;",","")</f>
+        <v>-7.11364603926745,</v>
       </c>
       <c r="C147" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D154&amp;"},","}}")</f>
@@ -15676,8 +15675,8 @@
         <v>{7.24999999999998,</v>
       </c>
       <c r="B148" t="str">
-        <f>IF(Sheet1!F155=0,","&amp;Sheet1!C155&amp;",","")</f>
-        <v>,-6.84050182915476,</v>
+        <f>IF(Sheet1!F155=0,Sheet1!C155&amp;",","")</f>
+        <v>-6.84050182915476,</v>
       </c>
       <c r="C148" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D155&amp;"},","}}")</f>
@@ -15690,8 +15689,8 @@
         <v>{7.29999999999998,</v>
       </c>
       <c r="B149" t="str">
-        <f>IF(Sheet1!F156=0,","&amp;Sheet1!C156&amp;",","")</f>
-        <v>,-6.55740971823208,</v>
+        <f>IF(Sheet1!F156=0,Sheet1!C156&amp;",","")</f>
+        <v>-6.55740971823208,</v>
       </c>
       <c r="C149" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D156&amp;"},","}}")</f>
@@ -15704,8 +15703,8 @@
         <v>{7.34999999999998,</v>
       </c>
       <c r="B150" t="str">
-        <f>IF(Sheet1!F157=0,","&amp;Sheet1!C157&amp;",","")</f>
-        <v>,-6.26478139738259,</v>
+        <f>IF(Sheet1!F157=0,Sheet1!C157&amp;",","")</f>
+        <v>-6.26478139738259,</v>
       </c>
       <c r="C150" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D157&amp;"},","}}")</f>
@@ -15718,8 +15717,8 @@
         <v>{7.39999999999998,</v>
       </c>
       <c r="B151" t="str">
-        <f>IF(Sheet1!F158=0,","&amp;Sheet1!C158&amp;",","")</f>
-        <v>,-5.96304242566362,</v>
+        <f>IF(Sheet1!F158=0,Sheet1!C158&amp;",","")</f>
+        <v>-5.96304242566362,</v>
       </c>
       <c r="C151" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D158&amp;"},","}}")</f>
@@ -15732,8 +15731,8 @@
         <v>{7.44999999999998,</v>
       </c>
       <c r="B152" t="str">
-        <f>IF(Sheet1!F159=0,","&amp;Sheet1!C159&amp;",","")</f>
-        <v>,-5.65263161143107,</v>
+        <f>IF(Sheet1!F159=0,Sheet1!C159&amp;",","")</f>
+        <v>-5.65263161143107,</v>
       </c>
       <c r="C152" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D159&amp;"},","}}")</f>
@@ -15746,8 +15745,8 @@
         <v>{7.49999999999998,</v>
       </c>
       <c r="B153" t="str">
-        <f>IF(Sheet1!F160=0,","&amp;Sheet1!C160&amp;",","")</f>
-        <v>,-5.33400037419588,</v>
+        <f>IF(Sheet1!F160=0,Sheet1!C160&amp;",","")</f>
+        <v>-5.33400037419588,</v>
       </c>
       <c r="C153" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D160&amp;"},","}}")</f>
@@ -15760,8 +15759,8 @@
         <v>{7.54999999999998,</v>
       </c>
       <c r="B154" t="str">
-        <f>IF(Sheet1!F161=0,","&amp;Sheet1!C161&amp;",","")</f>
-        <v>,-5.00761208814055,</v>
+        <f>IF(Sheet1!F161=0,Sheet1!C161&amp;",","")</f>
+        <v>-5.00761208814055,</v>
       </c>
       <c r="C154" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D161&amp;"},","}}")</f>
@@ -15774,8 +15773,8 @@
         <v>{7.59999999999998,</v>
       </c>
       <c r="B155" t="str">
-        <f>IF(Sheet1!F162=0,","&amp;Sheet1!C162&amp;",","")</f>
-        <v>,-4.6739414082504,</v>
+        <f>IF(Sheet1!F162=0,Sheet1!C162&amp;",","")</f>
+        <v>-4.6739414082504,</v>
       </c>
       <c r="C155" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D162&amp;"},","}}")</f>
@@ -15788,8 +15787,8 @@
         <v>{7.64999999999998,</v>
       </c>
       <c r="B156" t="str">
-        <f>IF(Sheet1!F163=0,","&amp;Sheet1!C163&amp;",","")</f>
-        <v>,-4.33347358003951,</v>
+        <f>IF(Sheet1!F163=0,Sheet1!C163&amp;",","")</f>
+        <v>-4.33347358003951,</v>
       </c>
       <c r="C156" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D163&amp;"},","}}")</f>
@@ -15802,8 +15801,8 @@
         <v>{7.69999999999998,</v>
       </c>
       <c r="B157" t="str">
-        <f>IF(Sheet1!F164=0,","&amp;Sheet1!C164&amp;",","")</f>
-        <v>,-3.98670373387531,</v>
+        <f>IF(Sheet1!F164=0,Sheet1!C164&amp;",","")</f>
+        <v>-3.98670373387531,</v>
       </c>
       <c r="C157" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D164&amp;"},","}}")</f>
@@ -15816,8 +15815,8 @@
         <v>{7.74999999999998,</v>
       </c>
       <c r="B158" t="str">
-        <f>IF(Sheet1!F165=0,","&amp;Sheet1!C165&amp;",","")</f>
-        <v>,-3.63413616492791,</v>
+        <f>IF(Sheet1!F165=0,Sheet1!C165&amp;",","")</f>
+        <v>-3.63413616492791,</v>
       </c>
       <c r="C158" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D165&amp;"},","}}")</f>
@@ -15830,8 +15829,8 @@
         <v>{7.79999999999998,</v>
       </c>
       <c r="B159" t="str">
-        <f>IF(Sheet1!F166=0,","&amp;Sheet1!C166&amp;",","")</f>
-        <v>,-3.2762835997914,</v>
+        <f>IF(Sheet1!F166=0,Sheet1!C166&amp;",","")</f>
+        <v>-3.2762835997914,</v>
       </c>
       <c r="C159" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D166&amp;"},","}}")</f>
@@ -15844,8 +15843,8 @@
         <v>{7.84999999999998,</v>
       </c>
       <c r="B160" t="str">
-        <f>IF(Sheet1!F167=0,","&amp;Sheet1!C167&amp;",","")</f>
-        <v>,-2.91366645084362,</v>
+        <f>IF(Sheet1!F167=0,Sheet1!C167&amp;",","")</f>
+        <v>-2.91366645084362,</v>
       </c>
       <c r="C160" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D167&amp;"},","}}")</f>
@@ -15858,8 +15857,8 @@
         <v>{7.89999999999998,</v>
       </c>
       <c r="B161" t="str">
-        <f>IF(Sheet1!F168=0,","&amp;Sheet1!C168&amp;",","")</f>
-        <v>,-2.54681205942878,</v>
+        <f>IF(Sheet1!F168=0,Sheet1!C168&amp;",","")</f>
+        <v>-2.54681205942878,</v>
       </c>
       <c r="C161" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D168&amp;"},","}}")</f>
@@ -15872,8 +15871,8 @@
         <v>{7.94999999999998,</v>
       </c>
       <c r="B162" t="str">
-        <f>IF(Sheet1!F169=0,","&amp;Sheet1!C169&amp;",","")</f>
-        <v>,-2.17625392896356,</v>
+        <f>IF(Sheet1!F169=0,Sheet1!C169&amp;",","")</f>
+        <v>-2.17625392896356,</v>
       </c>
       <c r="C162" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D169&amp;"},","}}")</f>
@@ -15886,8 +15885,8 @@
         <v>{7.99999999999998,</v>
       </c>
       <c r="B163" t="str">
-        <f>IF(Sheet1!F170=0,","&amp;Sheet1!C170&amp;",","")</f>
-        <v>,-1.80253094908182,</v>
+        <f>IF(Sheet1!F170=0,Sheet1!C170&amp;",","")</f>
+        <v>-1.80253094908182,</v>
       </c>
       <c r="C163" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D170&amp;"},","}}")</f>
@@ -15900,8 +15899,8 @@
         <v>{8.04999999999998,</v>
       </c>
       <c r="B164" t="str">
-        <f>IF(Sheet1!F171=0,","&amp;Sheet1!C171&amp;",","")</f>
-        <v>,-1.42618661194644,</v>
+        <f>IF(Sheet1!F171=0,Sheet1!C171&amp;",","")</f>
+        <v>-1.42618661194644,</v>
       </c>
       <c r="C164" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D171&amp;"},","}}")</f>
@@ -15914,8 +15913,8 @@
         <v>{8.09999999999998,</v>
       </c>
       <c r="B165" t="str">
-        <f>IF(Sheet1!F172=0,","&amp;Sheet1!C172&amp;",","")</f>
-        <v>,-1.04776822186778,</v>
+        <f>IF(Sheet1!F172=0,Sheet1!C172&amp;",","")</f>
+        <v>-1.04776822186778,</v>
       </c>
       <c r="C165" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D172&amp;"},","}}")</f>
@@ -15928,8 +15927,8 @@
         <v>{8.14999999999998,</v>
       </c>
       <c r="B166" t="str">
-        <f>IF(Sheet1!F173=0,","&amp;Sheet1!C173&amp;",","")</f>
-        <v>,-0.667826099378355,</v>
+        <f>IF(Sheet1!F173=0,Sheet1!C173&amp;",","")</f>
+        <v>-0.667826099378355,</v>
       </c>
       <c r="C166" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D173&amp;"},","}}")</f>
@@ -15942,8 +15941,8 @@
         <v>{8.19999999999998,</v>
       </c>
       <c r="B167" t="str">
-        <f>IF(Sheet1!F174=0,","&amp;Sheet1!C174&amp;",","")</f>
-        <v>,-0.286912780921018,</v>
+        <f>IF(Sheet1!F174=0,Sheet1!C174&amp;",","")</f>
+        <v>-0.286912780921018,</v>
       </c>
       <c r="C167" t="str">
         <f>IF(Sheet1!$F$10=0,Sheet1!D174&amp;"},","}}")</f>
@@ -15956,7 +15955,7 @@
         <v/>
       </c>
       <c r="B168" t="str">
-        <f>IF(Sheet1!F175=0,","&amp;Sheet1!C175&amp;",","")</f>
+        <f>IF(Sheet1!F175=0,Sheet1!C175&amp;",","")</f>
         <v/>
       </c>
       <c r="C168" t="str">
@@ -15970,7 +15969,7 @@
         <v/>
       </c>
       <c r="B169" t="str">
-        <f>IF(Sheet1!F176=0,","&amp;Sheet1!C176&amp;",","")</f>
+        <f>IF(Sheet1!F176=0,Sheet1!C176&amp;",","")</f>
         <v/>
       </c>
       <c r="C169" t="str">
@@ -15984,7 +15983,7 @@
         <v/>
       </c>
       <c r="B170" t="str">
-        <f>IF(Sheet1!F177=0,","&amp;Sheet1!C177&amp;",","")</f>
+        <f>IF(Sheet1!F177=0,Sheet1!C177&amp;",","")</f>
         <v/>
       </c>
       <c r="C170" t="str">
@@ -15998,7 +15997,7 @@
         <v/>
       </c>
       <c r="B171" t="str">
-        <f>IF(Sheet1!F178=0,","&amp;Sheet1!C178&amp;",","")</f>
+        <f>IF(Sheet1!F178=0,Sheet1!C178&amp;",","")</f>
         <v/>
       </c>
       <c r="C171" t="str">
@@ -16012,7 +16011,7 @@
         <v/>
       </c>
       <c r="B172" t="str">
-        <f>IF(Sheet1!F179=0,","&amp;Sheet1!C179&amp;",","")</f>
+        <f>IF(Sheet1!F179=0,Sheet1!C179&amp;",","")</f>
         <v/>
       </c>
       <c r="C172" t="str">
@@ -16026,7 +16025,7 @@
         <v/>
       </c>
       <c r="B173" t="str">
-        <f>IF(Sheet1!F180=0,","&amp;Sheet1!C180&amp;",","")</f>
+        <f>IF(Sheet1!F180=0,Sheet1!C180&amp;",","")</f>
         <v/>
       </c>
       <c r="C173" t="str">
@@ -16040,7 +16039,7 @@
         <v/>
       </c>
       <c r="B174" t="str">
-        <f>IF(Sheet1!F181=0,","&amp;Sheet1!C181&amp;",","")</f>
+        <f>IF(Sheet1!F181=0,Sheet1!C181&amp;",","")</f>
         <v/>
       </c>
       <c r="C174" t="str">
@@ -16054,7 +16053,7 @@
         <v/>
       </c>
       <c r="B175" t="str">
-        <f>IF(Sheet1!F182=0,","&amp;Sheet1!C182&amp;",","")</f>
+        <f>IF(Sheet1!F182=0,Sheet1!C182&amp;",","")</f>
         <v/>
       </c>
       <c r="C175" t="str">
@@ -16068,7 +16067,7 @@
         <v/>
       </c>
       <c r="B176" t="str">
-        <f>IF(Sheet1!F183=0,","&amp;Sheet1!C183&amp;",","")</f>
+        <f>IF(Sheet1!F183=0,Sheet1!C183&amp;",","")</f>
         <v/>
       </c>
       <c r="C176" t="str">
@@ -16082,7 +16081,7 @@
         <v/>
       </c>
       <c r="B177" t="str">
-        <f>IF(Sheet1!F184=0,","&amp;Sheet1!C184&amp;",","")</f>
+        <f>IF(Sheet1!F184=0,Sheet1!C184&amp;",","")</f>
         <v/>
       </c>
       <c r="C177" t="str">
@@ -16096,7 +16095,7 @@
         <v/>
       </c>
       <c r="B178" t="str">
-        <f>IF(Sheet1!F185=0,","&amp;Sheet1!C185&amp;",","")</f>
+        <f>IF(Sheet1!F185=0,Sheet1!C185&amp;",","")</f>
         <v/>
       </c>
       <c r="C178" t="str">
@@ -16110,7 +16109,7 @@
         <v/>
       </c>
       <c r="B179" t="str">
-        <f>IF(Sheet1!F186=0,","&amp;Sheet1!C186&amp;",","")</f>
+        <f>IF(Sheet1!F186=0,Sheet1!C186&amp;",","")</f>
         <v/>
       </c>
       <c r="C179" t="str">
@@ -16124,7 +16123,7 @@
         <v/>
       </c>
       <c r="B180" t="str">
-        <f>IF(Sheet1!F187=0,","&amp;Sheet1!C187&amp;",","")</f>
+        <f>IF(Sheet1!F187=0,Sheet1!C187&amp;",","")</f>
         <v/>
       </c>
       <c r="C180" t="str">
@@ -16138,7 +16137,7 @@
         <v/>
       </c>
       <c r="B181" t="str">
-        <f>IF(Sheet1!F188=0,","&amp;Sheet1!C188&amp;",","")</f>
+        <f>IF(Sheet1!F188=0,Sheet1!C188&amp;",","")</f>
         <v/>
       </c>
       <c r="C181" t="str">
@@ -16152,7 +16151,7 @@
         <v/>
       </c>
       <c r="B182" t="str">
-        <f>IF(Sheet1!F189=0,","&amp;Sheet1!C189&amp;",","")</f>
+        <f>IF(Sheet1!F189=0,Sheet1!C189&amp;",","")</f>
         <v/>
       </c>
       <c r="C182" t="str">
@@ -16166,7 +16165,7 @@
         <v/>
       </c>
       <c r="B183" t="str">
-        <f>IF(Sheet1!F190=0,","&amp;Sheet1!C190&amp;",","")</f>
+        <f>IF(Sheet1!F190=0,Sheet1!C190&amp;",","")</f>
         <v/>
       </c>
       <c r="C183" t="str">
@@ -16180,7 +16179,7 @@
         <v/>
       </c>
       <c r="B184" t="str">
-        <f>IF(Sheet1!F191=0,","&amp;Sheet1!C191&amp;",","")</f>
+        <f>IF(Sheet1!F191=0,Sheet1!C191&amp;",","")</f>
         <v/>
       </c>
       <c r="C184" t="str">
@@ -16194,7 +16193,7 @@
         <v/>
       </c>
       <c r="B185" t="str">
-        <f>IF(Sheet1!F192=0,","&amp;Sheet1!C192&amp;",","")</f>
+        <f>IF(Sheet1!F192=0,Sheet1!C192&amp;",","")</f>
         <v/>
       </c>
       <c r="C185" t="str">
@@ -16208,7 +16207,7 @@
         <v/>
       </c>
       <c r="B186" t="str">
-        <f>IF(Sheet1!F193=0,","&amp;Sheet1!C193&amp;",","")</f>
+        <f>IF(Sheet1!F193=0,Sheet1!C193&amp;",","")</f>
         <v/>
       </c>
       <c r="C186" t="str">
@@ -16222,7 +16221,7 @@
         <v/>
       </c>
       <c r="B187" t="str">
-        <f>IF(Sheet1!F194=0,","&amp;Sheet1!C194&amp;",","")</f>
+        <f>IF(Sheet1!F194=0,Sheet1!C194&amp;",","")</f>
         <v/>
       </c>
       <c r="C187" t="str">
@@ -16236,7 +16235,7 @@
         <v/>
       </c>
       <c r="B188" t="str">
-        <f>IF(Sheet1!F195=0,","&amp;Sheet1!C195&amp;",","")</f>
+        <f>IF(Sheet1!F195=0,Sheet1!C195&amp;",","")</f>
         <v/>
       </c>
       <c r="C188" t="str">
@@ -16250,7 +16249,7 @@
         <v/>
       </c>
       <c r="B189" t="str">
-        <f>IF(Sheet1!F196=0,","&amp;Sheet1!C196&amp;",","")</f>
+        <f>IF(Sheet1!F196=0,Sheet1!C196&amp;",","")</f>
         <v/>
       </c>
       <c r="C189" t="str">
@@ -16264,7 +16263,7 @@
         <v/>
       </c>
       <c r="B190" t="str">
-        <f>IF(Sheet1!F197=0,","&amp;Sheet1!C197&amp;",","")</f>
+        <f>IF(Sheet1!F197=0,Sheet1!C197&amp;",","")</f>
         <v/>
       </c>
       <c r="C190" t="str">
@@ -16278,7 +16277,7 @@
         <v/>
       </c>
       <c r="B191" t="str">
-        <f>IF(Sheet1!F198=0,","&amp;Sheet1!C198&amp;",","")</f>
+        <f>IF(Sheet1!F198=0,Sheet1!C198&amp;",","")</f>
         <v/>
       </c>
       <c r="C191" t="str">
@@ -16292,7 +16291,7 @@
         <v/>
       </c>
       <c r="B192" t="str">
-        <f>IF(Sheet1!F199=0,","&amp;Sheet1!C199&amp;",","")</f>
+        <f>IF(Sheet1!F199=0,Sheet1!C199&amp;",","")</f>
         <v/>
       </c>
       <c r="C192" t="str">
@@ -16306,7 +16305,7 @@
         <v/>
       </c>
       <c r="B193" t="str">
-        <f>IF(Sheet1!F200=0,","&amp;Sheet1!C200&amp;",","")</f>
+        <f>IF(Sheet1!F200=0,Sheet1!C200&amp;",","")</f>
         <v/>
       </c>
       <c r="C193" t="str">
@@ -16320,7 +16319,7 @@
         <v/>
       </c>
       <c r="B194" t="str">
-        <f>IF(Sheet1!F201=0,","&amp;Sheet1!C201&amp;",","")</f>
+        <f>IF(Sheet1!F201=0,Sheet1!C201&amp;",","")</f>
         <v/>
       </c>
       <c r="C194" t="str">
@@ -16334,7 +16333,7 @@
         <v/>
       </c>
       <c r="B195" t="str">
-        <f>IF(Sheet1!F202=0,","&amp;Sheet1!C202&amp;",","")</f>
+        <f>IF(Sheet1!F202=0,Sheet1!C202&amp;",","")</f>
         <v/>
       </c>
       <c r="C195" t="str">
@@ -16348,7 +16347,7 @@
         <v/>
       </c>
       <c r="B196" t="str">
-        <f>IF(Sheet1!F203=0,","&amp;Sheet1!C203&amp;",","")</f>
+        <f>IF(Sheet1!F203=0,Sheet1!C203&amp;",","")</f>
         <v/>
       </c>
       <c r="C196" t="str">
@@ -16362,7 +16361,7 @@
         <v/>
       </c>
       <c r="B197" t="str">
-        <f>IF(Sheet1!F204=0,","&amp;Sheet1!C204&amp;",","")</f>
+        <f>IF(Sheet1!F204=0,Sheet1!C204&amp;",","")</f>
         <v/>
       </c>
       <c r="C197" t="str">
@@ -16376,7 +16375,7 @@
         <v/>
       </c>
       <c r="B198" t="str">
-        <f>IF(Sheet1!F205=0,","&amp;Sheet1!C205&amp;",","")</f>
+        <f>IF(Sheet1!F205=0,Sheet1!C205&amp;",","")</f>
         <v/>
       </c>
       <c r="C198" t="str">
@@ -16390,7 +16389,7 @@
         <v/>
       </c>
       <c r="B199" t="str">
-        <f>IF(Sheet1!F206=0,","&amp;Sheet1!C206&amp;",","")</f>
+        <f>IF(Sheet1!F206=0,Sheet1!C206&amp;",","")</f>
         <v/>
       </c>
       <c r="C199" t="str">
@@ -16404,7 +16403,7 @@
         <v/>
       </c>
       <c r="B200" t="str">
-        <f>IF(Sheet1!F207=0,","&amp;Sheet1!C207&amp;",","")</f>
+        <f>IF(Sheet1!F207=0,Sheet1!C207&amp;",","")</f>
         <v/>
       </c>
       <c r="C200" t="str">
@@ -16418,7 +16417,7 @@
         <v/>
       </c>
       <c r="B201" t="str">
-        <f>IF(Sheet1!F208=0,","&amp;Sheet1!C208&amp;",","")</f>
+        <f>IF(Sheet1!F208=0,Sheet1!C208&amp;",","")</f>
         <v/>
       </c>
       <c r="C201" t="str">
@@ -16432,7 +16431,7 @@
         <v/>
       </c>
       <c r="B202" t="str">
-        <f>IF(Sheet1!F209=0,","&amp;Sheet1!C209&amp;",","")</f>
+        <f>IF(Sheet1!F209=0,Sheet1!C209&amp;",","")</f>
         <v/>
       </c>
       <c r="C202" t="str">
@@ -16446,7 +16445,7 @@
         <v/>
       </c>
       <c r="B203" t="str">
-        <f>IF(Sheet1!F210=0,","&amp;Sheet1!C210&amp;",","")</f>
+        <f>IF(Sheet1!F210=0,Sheet1!C210&amp;",","")</f>
         <v/>
       </c>
       <c r="C203" t="str">
@@ -16460,7 +16459,7 @@
         <v/>
       </c>
       <c r="B204" t="str">
-        <f>IF(Sheet1!F211=0,","&amp;Sheet1!C211&amp;",","")</f>
+        <f>IF(Sheet1!F211=0,Sheet1!C211&amp;",","")</f>
         <v/>
       </c>
       <c r="C204" t="str">
@@ -16474,7 +16473,7 @@
         <v/>
       </c>
       <c r="B205" t="str">
-        <f>IF(Sheet1!F212=0,","&amp;Sheet1!C212&amp;",","")</f>
+        <f>IF(Sheet1!F212=0,Sheet1!C212&amp;",","")</f>
         <v/>
       </c>
       <c r="C205" t="str">
@@ -16488,7 +16487,7 @@
         <v/>
       </c>
       <c r="B206" t="str">
-        <f>IF(Sheet1!F213=0,","&amp;Sheet1!C213&amp;",","")</f>
+        <f>IF(Sheet1!F213=0,Sheet1!C213&amp;",","")</f>
         <v/>
       </c>
       <c r="C206" t="str">
@@ -16502,7 +16501,7 @@
         <v/>
       </c>
       <c r="B207" t="str">
-        <f>IF(Sheet1!F214=0,","&amp;Sheet1!C214&amp;",","")</f>
+        <f>IF(Sheet1!F214=0,Sheet1!C214&amp;",","")</f>
         <v/>
       </c>
       <c r="C207" t="str">
@@ -16516,7 +16515,7 @@
         <v/>
       </c>
       <c r="B208" t="str">
-        <f>IF(Sheet1!F215=0,","&amp;Sheet1!C215&amp;",","")</f>
+        <f>IF(Sheet1!F215=0,Sheet1!C215&amp;",","")</f>
         <v/>
       </c>
       <c r="C208" t="str">
@@ -16530,7 +16529,7 @@
         <v/>
       </c>
       <c r="B209" t="str">
-        <f>IF(Sheet1!F216=0,","&amp;Sheet1!C216&amp;",","")</f>
+        <f>IF(Sheet1!F216=0,Sheet1!C216&amp;",","")</f>
         <v/>
       </c>
       <c r="C209" t="str">
@@ -16544,7 +16543,7 @@
         <v/>
       </c>
       <c r="B210" t="str">
-        <f>IF(Sheet1!F217=0,","&amp;Sheet1!C217&amp;",","")</f>
+        <f>IF(Sheet1!F217=0,Sheet1!C217&amp;",","")</f>
         <v/>
       </c>
       <c r="C210" t="str">
@@ -16558,7 +16557,7 @@
         <v/>
       </c>
       <c r="B211" t="str">
-        <f>IF(Sheet1!F218=0,","&amp;Sheet1!C218&amp;",","")</f>
+        <f>IF(Sheet1!F218=0,Sheet1!C218&amp;",","")</f>
         <v/>
       </c>
       <c r="C211" t="str">
@@ -16572,7 +16571,7 @@
         <v/>
       </c>
       <c r="B212" t="str">
-        <f>IF(Sheet1!F219=0,","&amp;Sheet1!C219&amp;",","")</f>
+        <f>IF(Sheet1!F219=0,Sheet1!C219&amp;",","")</f>
         <v/>
       </c>
       <c r="C212" t="str">
@@ -16586,7 +16585,7 @@
         <v/>
       </c>
       <c r="B213" t="str">
-        <f>IF(Sheet1!F220=0,","&amp;Sheet1!C220&amp;",","")</f>
+        <f>IF(Sheet1!F220=0,Sheet1!C220&amp;",","")</f>
         <v/>
       </c>
       <c r="C213" t="str">
@@ -16600,7 +16599,7 @@
         <v/>
       </c>
       <c r="B214" t="str">
-        <f>IF(Sheet1!F221=0,","&amp;Sheet1!C221&amp;",","")</f>
+        <f>IF(Sheet1!F221=0,Sheet1!C221&amp;",","")</f>
         <v/>
       </c>
       <c r="C214" t="str">
@@ -16614,7 +16613,7 @@
         <v/>
       </c>
       <c r="B215" t="str">
-        <f>IF(Sheet1!F222=0,","&amp;Sheet1!C222&amp;",","")</f>
+        <f>IF(Sheet1!F222=0,Sheet1!C222&amp;",","")</f>
         <v/>
       </c>
       <c r="C215" t="str">
@@ -16628,7 +16627,7 @@
         <v/>
       </c>
       <c r="B216" t="str">
-        <f>IF(Sheet1!F223=0,","&amp;Sheet1!C223&amp;",","")</f>
+        <f>IF(Sheet1!F223=0,Sheet1!C223&amp;",","")</f>
         <v/>
       </c>
       <c r="C216" t="str">
@@ -16642,7 +16641,7 @@
         <v/>
       </c>
       <c r="B217" t="str">
-        <f>IF(Sheet1!F224=0,","&amp;Sheet1!C224&amp;",","")</f>
+        <f>IF(Sheet1!F224=0,Sheet1!C224&amp;",","")</f>
         <v/>
       </c>
       <c r="C217" t="str">
@@ -16656,7 +16655,7 @@
         <v/>
       </c>
       <c r="B218" t="str">
-        <f>IF(Sheet1!F225=0,","&amp;Sheet1!C225&amp;",","")</f>
+        <f>IF(Sheet1!F225=0,Sheet1!C225&amp;",","")</f>
         <v/>
       </c>
       <c r="C218" t="str">
@@ -16670,7 +16669,7 @@
         <v/>
       </c>
       <c r="B219" t="str">
-        <f>IF(Sheet1!F226=0,","&amp;Sheet1!C226&amp;",","")</f>
+        <f>IF(Sheet1!F226=0,Sheet1!C226&amp;",","")</f>
         <v/>
       </c>
       <c r="C219" t="str">
@@ -16684,7 +16683,7 @@
         <v/>
       </c>
       <c r="B220" t="str">
-        <f>IF(Sheet1!F227=0,","&amp;Sheet1!C227&amp;",","")</f>
+        <f>IF(Sheet1!F227=0,Sheet1!C227&amp;",","")</f>
         <v/>
       </c>
       <c r="C220" t="str">
@@ -16698,7 +16697,7 @@
         <v/>
       </c>
       <c r="B221" t="str">
-        <f>IF(Sheet1!F228=0,","&amp;Sheet1!C228&amp;",","")</f>
+        <f>IF(Sheet1!F228=0,Sheet1!C228&amp;",","")</f>
         <v/>
       </c>
       <c r="C221" t="str">
@@ -16712,7 +16711,7 @@
         <v/>
       </c>
       <c r="B222" t="str">
-        <f>IF(Sheet1!F229=0,","&amp;Sheet1!C229&amp;",","")</f>
+        <f>IF(Sheet1!F229=0,Sheet1!C229&amp;",","")</f>
         <v/>
       </c>
       <c r="C222" t="str">
@@ -16726,7 +16725,7 @@
         <v/>
       </c>
       <c r="B223" t="str">
-        <f>IF(Sheet1!F230=0,","&amp;Sheet1!C230&amp;",","")</f>
+        <f>IF(Sheet1!F230=0,Sheet1!C230&amp;",","")</f>
         <v/>
       </c>
       <c r="C223" t="str">
@@ -16740,7 +16739,7 @@
         <v/>
       </c>
       <c r="B224" t="str">
-        <f>IF(Sheet1!F231=0,","&amp;Sheet1!C231&amp;",","")</f>
+        <f>IF(Sheet1!F231=0,Sheet1!C231&amp;",","")</f>
         <v/>
       </c>
       <c r="C224" t="str">
@@ -16754,7 +16753,7 @@
         <v/>
       </c>
       <c r="B225" t="str">
-        <f>IF(Sheet1!F232=0,","&amp;Sheet1!C232&amp;",","")</f>
+        <f>IF(Sheet1!F232=0,Sheet1!C232&amp;",","")</f>
         <v/>
       </c>
       <c r="C225" t="str">
@@ -16768,7 +16767,7 @@
         <v/>
       </c>
       <c r="B226" t="str">
-        <f>IF(Sheet1!F233=0,","&amp;Sheet1!C233&amp;",","")</f>
+        <f>IF(Sheet1!F233=0,Sheet1!C233&amp;",","")</f>
         <v/>
       </c>
       <c r="C226" t="str">
@@ -16782,7 +16781,7 @@
         <v/>
       </c>
       <c r="B227" t="str">
-        <f>IF(Sheet1!F234=0,","&amp;Sheet1!C234&amp;",","")</f>
+        <f>IF(Sheet1!F234=0,Sheet1!C234&amp;",","")</f>
         <v/>
       </c>
       <c r="C227" t="str">
@@ -16796,7 +16795,7 @@
         <v/>
       </c>
       <c r="B228" t="str">
-        <f>IF(Sheet1!F235=0,","&amp;Sheet1!C235&amp;",","")</f>
+        <f>IF(Sheet1!F235=0,Sheet1!C235&amp;",","")</f>
         <v/>
       </c>
       <c r="C228" t="str">
@@ -16810,7 +16809,7 @@
         <v/>
       </c>
       <c r="B229" t="str">
-        <f>IF(Sheet1!F236=0,","&amp;Sheet1!C236&amp;",","")</f>
+        <f>IF(Sheet1!F236=0,Sheet1!C236&amp;",","")</f>
         <v/>
       </c>
       <c r="C229" t="str">
@@ -16824,7 +16823,7 @@
         <v/>
       </c>
       <c r="B230" t="str">
-        <f>IF(Sheet1!F237=0,","&amp;Sheet1!C237&amp;",","")</f>
+        <f>IF(Sheet1!F237=0,Sheet1!C237&amp;",","")</f>
         <v/>
       </c>
       <c r="C230" t="str">
@@ -16838,7 +16837,7 @@
         <v/>
       </c>
       <c r="B231" t="str">
-        <f>IF(Sheet1!F238=0,","&amp;Sheet1!C238&amp;",","")</f>
+        <f>IF(Sheet1!F238=0,Sheet1!C238&amp;",","")</f>
         <v/>
       </c>
       <c r="C231" t="str">
@@ -16852,7 +16851,7 @@
         <v/>
       </c>
       <c r="B232" t="str">
-        <f>IF(Sheet1!F239=0,","&amp;Sheet1!C239&amp;",","")</f>
+        <f>IF(Sheet1!F239=0,Sheet1!C239&amp;",","")</f>
         <v/>
       </c>
       <c r="C232" t="str">
@@ -16866,7 +16865,7 @@
         <v/>
       </c>
       <c r="B233" t="str">
-        <f>IF(Sheet1!F240=0,","&amp;Sheet1!C240&amp;",","")</f>
+        <f>IF(Sheet1!F240=0,Sheet1!C240&amp;",","")</f>
         <v/>
       </c>
       <c r="C233" t="str">
@@ -16880,7 +16879,7 @@
         <v/>
       </c>
       <c r="B234" t="str">
-        <f>IF(Sheet1!F241=0,","&amp;Sheet1!C241&amp;",","")</f>
+        <f>IF(Sheet1!F241=0,Sheet1!C241&amp;",","")</f>
         <v/>
       </c>
       <c r="C234" t="str">
@@ -16894,7 +16893,7 @@
         <v/>
       </c>
       <c r="B235" t="str">
-        <f>IF(Sheet1!F242=0,","&amp;Sheet1!C242&amp;",","")</f>
+        <f>IF(Sheet1!F242=0,Sheet1!C242&amp;",","")</f>
         <v/>
       </c>
       <c r="C235" t="str">
@@ -16908,7 +16907,7 @@
         <v/>
       </c>
       <c r="B236" t="str">
-        <f>IF(Sheet1!F243=0,","&amp;Sheet1!C243&amp;",","")</f>
+        <f>IF(Sheet1!F243=0,Sheet1!C243&amp;",","")</f>
         <v/>
       </c>
       <c r="C236" t="str">
@@ -16922,7 +16921,7 @@
         <v/>
       </c>
       <c r="B237" t="str">
-        <f>IF(Sheet1!F244=0,","&amp;Sheet1!C244&amp;",","")</f>
+        <f>IF(Sheet1!F244=0,Sheet1!C244&amp;",","")</f>
         <v/>
       </c>
       <c r="C237" t="str">
@@ -16936,7 +16935,7 @@
         <v/>
       </c>
       <c r="B238" t="str">
-        <f>IF(Sheet1!F245=0,","&amp;Sheet1!C245&amp;",","")</f>
+        <f>IF(Sheet1!F245=0,Sheet1!C245&amp;",","")</f>
         <v/>
       </c>
       <c r="C238" t="str">
@@ -16950,7 +16949,7 @@
         <v/>
       </c>
       <c r="B239" t="str">
-        <f>IF(Sheet1!F246=0,","&amp;Sheet1!C246&amp;",","")</f>
+        <f>IF(Sheet1!F246=0,Sheet1!C246&amp;",","")</f>
         <v/>
       </c>
       <c r="C239" t="str">
@@ -16964,7 +16963,7 @@
         <v/>
       </c>
       <c r="B240" t="str">
-        <f>IF(Sheet1!F247=0,","&amp;Sheet1!C247&amp;",","")</f>
+        <f>IF(Sheet1!F247=0,Sheet1!C247&amp;",","")</f>
         <v/>
       </c>
       <c r="C240" t="str">
@@ -16978,7 +16977,7 @@
         <v/>
       </c>
       <c r="B241" t="str">
-        <f>IF(Sheet1!F248=0,","&amp;Sheet1!C248&amp;",","")</f>
+        <f>IF(Sheet1!F248=0,Sheet1!C248&amp;",","")</f>
         <v/>
       </c>
       <c r="C241" t="str">
@@ -16992,7 +16991,7 @@
         <v/>
       </c>
       <c r="B242" t="str">
-        <f>IF(Sheet1!F249=0,","&amp;Sheet1!C249&amp;",","")</f>
+        <f>IF(Sheet1!F249=0,Sheet1!C249&amp;",","")</f>
         <v/>
       </c>
       <c r="C242" t="str">
@@ -17006,7 +17005,7 @@
         <v/>
       </c>
       <c r="B243" t="str">
-        <f>IF(Sheet1!F250=0,","&amp;Sheet1!C250&amp;",","")</f>
+        <f>IF(Sheet1!F250=0,Sheet1!C250&amp;",","")</f>
         <v/>
       </c>
       <c r="C243" t="str">
@@ -17020,7 +17019,7 @@
         <v/>
       </c>
       <c r="B244" t="str">
-        <f>IF(Sheet1!F251=0,","&amp;Sheet1!C251&amp;",","")</f>
+        <f>IF(Sheet1!F251=0,Sheet1!C251&amp;",","")</f>
         <v/>
       </c>
       <c r="C244" t="str">
@@ -17034,7 +17033,7 @@
         <v/>
       </c>
       <c r="B245" t="str">
-        <f>IF(Sheet1!F252=0,","&amp;Sheet1!C252&amp;",","")</f>
+        <f>IF(Sheet1!F252=0,Sheet1!C252&amp;",","")</f>
         <v/>
       </c>
       <c r="C245" t="str">
@@ -17048,7 +17047,7 @@
         <v/>
       </c>
       <c r="B246" t="str">
-        <f>IF(Sheet1!F253=0,","&amp;Sheet1!C253&amp;",","")</f>
+        <f>IF(Sheet1!F253=0,Sheet1!C253&amp;",","")</f>
         <v/>
       </c>
       <c r="C246" t="str">
@@ -17062,7 +17061,7 @@
         <v/>
       </c>
       <c r="B247" t="str">
-        <f>IF(Sheet1!F254=0,","&amp;Sheet1!C254&amp;",","")</f>
+        <f>IF(Sheet1!F254=0,Sheet1!C254&amp;",","")</f>
         <v/>
       </c>
       <c r="C247" t="str">
@@ -17076,7 +17075,7 @@
         <v/>
       </c>
       <c r="B248" t="str">
-        <f>IF(Sheet1!F255=0,","&amp;Sheet1!C255&amp;",","")</f>
+        <f>IF(Sheet1!F255=0,Sheet1!C255&amp;",","")</f>
         <v/>
       </c>
       <c r="C248" t="str">
@@ -17090,7 +17089,7 @@
         <v/>
       </c>
       <c r="B249" t="str">
-        <f>IF(Sheet1!F256=0,","&amp;Sheet1!C256&amp;",","")</f>
+        <f>IF(Sheet1!F256=0,Sheet1!C256&amp;",","")</f>
         <v/>
       </c>
       <c r="C249" t="str">
@@ -17104,7 +17103,7 @@
         <v/>
       </c>
       <c r="B250" t="str">
-        <f>IF(Sheet1!F257=0,","&amp;Sheet1!C257&amp;",","")</f>
+        <f>IF(Sheet1!F257=0,Sheet1!C257&amp;",","")</f>
         <v/>
       </c>
       <c r="C250" t="str">
@@ -17118,7 +17117,7 @@
         <v/>
       </c>
       <c r="B251" t="str">
-        <f>IF(Sheet1!F258=0,","&amp;Sheet1!C258&amp;",","")</f>
+        <f>IF(Sheet1!F258=0,Sheet1!C258&amp;",","")</f>
         <v/>
       </c>
       <c r="C251" t="str">
@@ -17132,7 +17131,7 @@
         <v/>
       </c>
       <c r="B252" t="str">
-        <f>IF(Sheet1!F259=0,","&amp;Sheet1!C259&amp;",","")</f>
+        <f>IF(Sheet1!F259=0,Sheet1!C259&amp;",","")</f>
         <v/>
       </c>
       <c r="C252" t="str">
@@ -17146,7 +17145,7 @@
         <v/>
       </c>
       <c r="B253" t="str">
-        <f>IF(Sheet1!F260=0,","&amp;Sheet1!C260&amp;",","")</f>
+        <f>IF(Sheet1!F260=0,Sheet1!C260&amp;",","")</f>
         <v/>
       </c>
       <c r="C253" t="str">
@@ -17160,7 +17159,7 @@
         <v/>
       </c>
       <c r="B254" t="str">
-        <f>IF(Sheet1!F261=0,","&amp;Sheet1!C261&amp;",","")</f>
+        <f>IF(Sheet1!F261=0,Sheet1!C261&amp;",","")</f>
         <v/>
       </c>
       <c r="C254" t="str">
@@ -17174,7 +17173,7 @@
         <v/>
       </c>
       <c r="B255" t="str">
-        <f>IF(Sheet1!F262=0,","&amp;Sheet1!C262&amp;",","")</f>
+        <f>IF(Sheet1!F262=0,Sheet1!C262&amp;",","")</f>
         <v/>
       </c>
       <c r="C255" t="str">
@@ -17188,7 +17187,7 @@
         <v/>
       </c>
       <c r="B256" t="str">
-        <f>IF(Sheet1!F263=0,","&amp;Sheet1!C263&amp;",","")</f>
+        <f>IF(Sheet1!F263=0,Sheet1!C263&amp;",","")</f>
         <v/>
       </c>
       <c r="C256" t="str">
@@ -17202,7 +17201,7 @@
         <v/>
       </c>
       <c r="B257" t="str">
-        <f>IF(Sheet1!F264=0,","&amp;Sheet1!C264&amp;",","")</f>
+        <f>IF(Sheet1!F264=0,Sheet1!C264&amp;",","")</f>
         <v/>
       </c>
       <c r="C257" t="str">
@@ -17216,7 +17215,7 @@
         <v/>
       </c>
       <c r="B258" t="str">
-        <f>IF(Sheet1!F265=0,","&amp;Sheet1!C265&amp;",","")</f>
+        <f>IF(Sheet1!F265=0,Sheet1!C265&amp;",","")</f>
         <v/>
       </c>
       <c r="C258" t="str">
@@ -17230,7 +17229,7 @@
         <v/>
       </c>
       <c r="B259" t="str">
-        <f>IF(Sheet1!F266=0,","&amp;Sheet1!C266&amp;",","")</f>
+        <f>IF(Sheet1!F266=0,Sheet1!C266&amp;",","")</f>
         <v/>
       </c>
       <c r="C259" t="str">
@@ -17244,7 +17243,7 @@
         <v/>
       </c>
       <c r="B260" t="str">
-        <f>IF(Sheet1!F267=0,","&amp;Sheet1!C267&amp;",","")</f>
+        <f>IF(Sheet1!F267=0,Sheet1!C267&amp;",","")</f>
         <v/>
       </c>
       <c r="C260" t="str">
@@ -17258,7 +17257,7 @@
         <v/>
       </c>
       <c r="B261" t="str">
-        <f>IF(Sheet1!F268=0,","&amp;Sheet1!C268&amp;",","")</f>
+        <f>IF(Sheet1!F268=0,Sheet1!C268&amp;",","")</f>
         <v/>
       </c>
       <c r="C261" t="str">
@@ -17272,7 +17271,7 @@
         <v/>
       </c>
       <c r="B262" t="str">
-        <f>IF(Sheet1!F269=0,","&amp;Sheet1!C269&amp;",","")</f>
+        <f>IF(Sheet1!F269=0,Sheet1!C269&amp;",","")</f>
         <v/>
       </c>
       <c r="C262" t="str">
@@ -17286,7 +17285,7 @@
         <v/>
       </c>
       <c r="B263" t="str">
-        <f>IF(Sheet1!F270=0,","&amp;Sheet1!C270&amp;",","")</f>
+        <f>IF(Sheet1!F270=0,Sheet1!C270&amp;",","")</f>
         <v/>
       </c>
       <c r="C263" t="str">
@@ -17300,7 +17299,7 @@
         <v/>
       </c>
       <c r="B264" t="str">
-        <f>IF(Sheet1!F271=0,","&amp;Sheet1!C271&amp;",","")</f>
+        <f>IF(Sheet1!F271=0,Sheet1!C271&amp;",","")</f>
         <v/>
       </c>
       <c r="C264" t="str">
@@ -17314,7 +17313,7 @@
         <v/>
       </c>
       <c r="B265" t="str">
-        <f>IF(Sheet1!F272=0,","&amp;Sheet1!C272&amp;",","")</f>
+        <f>IF(Sheet1!F272=0,Sheet1!C272&amp;",","")</f>
         <v/>
       </c>
       <c r="C265" t="str">
@@ -17328,7 +17327,7 @@
         <v/>
       </c>
       <c r="B266" t="str">
-        <f>IF(Sheet1!F273=0,","&amp;Sheet1!C273&amp;",","")</f>
+        <f>IF(Sheet1!F273=0,Sheet1!C273&amp;",","")</f>
         <v/>
       </c>
       <c r="C266" t="str">
@@ -17342,7 +17341,7 @@
         <v/>
       </c>
       <c r="B267" t="str">
-        <f>IF(Sheet1!F274=0,","&amp;Sheet1!C274&amp;",","")</f>
+        <f>IF(Sheet1!F274=0,Sheet1!C274&amp;",","")</f>
         <v/>
       </c>
       <c r="C267" t="str">
@@ -17356,7 +17355,7 @@
         <v/>
       </c>
       <c r="B268" t="str">
-        <f>IF(Sheet1!F275=0,","&amp;Sheet1!C275&amp;",","")</f>
+        <f>IF(Sheet1!F275=0,Sheet1!C275&amp;",","")</f>
         <v/>
       </c>
       <c r="C268" t="str">
@@ -17370,7 +17369,7 @@
         <v/>
       </c>
       <c r="B269" t="str">
-        <f>IF(Sheet1!F276=0,","&amp;Sheet1!C276&amp;",","")</f>
+        <f>IF(Sheet1!F276=0,Sheet1!C276&amp;",","")</f>
         <v/>
       </c>
       <c r="C269" t="str">
@@ -17384,7 +17383,7 @@
         <v/>
       </c>
       <c r="B270" t="str">
-        <f>IF(Sheet1!F277=0,","&amp;Sheet1!C277&amp;",","")</f>
+        <f>IF(Sheet1!F277=0,Sheet1!C277&amp;",","")</f>
         <v/>
       </c>
       <c r="C270" t="str">
@@ -17398,7 +17397,7 @@
         <v/>
       </c>
       <c r="B271" t="str">
-        <f>IF(Sheet1!F278=0,","&amp;Sheet1!C278&amp;",","")</f>
+        <f>IF(Sheet1!F278=0,Sheet1!C278&amp;",","")</f>
         <v/>
       </c>
       <c r="C271" t="str">
@@ -17412,7 +17411,7 @@
         <v/>
       </c>
       <c r="B272" t="str">
-        <f>IF(Sheet1!F279=0,","&amp;Sheet1!C279&amp;",","")</f>
+        <f>IF(Sheet1!F279=0,Sheet1!C279&amp;",","")</f>
         <v/>
       </c>
       <c r="C272" t="str">
@@ -17426,7 +17425,7 @@
         <v/>
       </c>
       <c r="B273" t="str">
-        <f>IF(Sheet1!F280=0,","&amp;Sheet1!C280&amp;",","")</f>
+        <f>IF(Sheet1!F280=0,Sheet1!C280&amp;",","")</f>
         <v/>
       </c>
       <c r="C273" t="str">
@@ -17440,7 +17439,7 @@
         <v/>
       </c>
       <c r="B274" t="str">
-        <f>IF(Sheet1!F281=0,","&amp;Sheet1!C281&amp;",","")</f>
+        <f>IF(Sheet1!F281=0,Sheet1!C281&amp;",","")</f>
         <v/>
       </c>
       <c r="C274" t="str">
@@ -17454,7 +17453,7 @@
         <v/>
       </c>
       <c r="B275" t="str">
-        <f>IF(Sheet1!F282=0,","&amp;Sheet1!C282&amp;",","")</f>
+        <f>IF(Sheet1!F282=0,Sheet1!C282&amp;",","")</f>
         <v/>
       </c>
       <c r="C275" t="str">
@@ -17468,7 +17467,7 @@
         <v/>
       </c>
       <c r="B276" t="str">
-        <f>IF(Sheet1!F283=0,","&amp;Sheet1!C283&amp;",","")</f>
+        <f>IF(Sheet1!F283=0,Sheet1!C283&amp;",","")</f>
         <v/>
       </c>
       <c r="C276" t="str">
@@ -17482,7 +17481,7 @@
         <v/>
       </c>
       <c r="B277" t="str">
-        <f>IF(Sheet1!F284=0,","&amp;Sheet1!C284&amp;",","")</f>
+        <f>IF(Sheet1!F284=0,Sheet1!C284&amp;",","")</f>
         <v/>
       </c>
       <c r="C277" t="str">
@@ -17496,7 +17495,7 @@
         <v/>
       </c>
       <c r="B278" t="str">
-        <f>IF(Sheet1!F285=0,","&amp;Sheet1!C285&amp;",","")</f>
+        <f>IF(Sheet1!F285=0,Sheet1!C285&amp;",","")</f>
         <v/>
       </c>
       <c r="C278" t="str">
@@ -17510,7 +17509,7 @@
         <v/>
       </c>
       <c r="B279" t="str">
-        <f>IF(Sheet1!F286=0,","&amp;Sheet1!C286&amp;",","")</f>
+        <f>IF(Sheet1!F286=0,Sheet1!C286&amp;",","")</f>
         <v/>
       </c>
       <c r="C279" t="str">
@@ -17524,7 +17523,7 @@
         <v/>
       </c>
       <c r="B280" t="str">
-        <f>IF(Sheet1!F287=0,","&amp;Sheet1!C287&amp;",","")</f>
+        <f>IF(Sheet1!F287=0,Sheet1!C287&amp;",","")</f>
         <v/>
       </c>
       <c r="C280" t="str">
@@ -17538,7 +17537,7 @@
         <v/>
       </c>
       <c r="B281" t="str">
-        <f>IF(Sheet1!F288=0,","&amp;Sheet1!C288&amp;",","")</f>
+        <f>IF(Sheet1!F288=0,Sheet1!C288&amp;",","")</f>
         <v/>
       </c>
       <c r="C281" t="str">
@@ -17552,7 +17551,7 @@
         <v/>
       </c>
       <c r="B282" t="str">
-        <f>IF(Sheet1!F289=0,","&amp;Sheet1!C289&amp;",","")</f>
+        <f>IF(Sheet1!F289=0,Sheet1!C289&amp;",","")</f>
         <v/>
       </c>
       <c r="C282" t="str">
@@ -17566,7 +17565,7 @@
         <v/>
       </c>
       <c r="B283" t="str">
-        <f>IF(Sheet1!F290=0,","&amp;Sheet1!C290&amp;",","")</f>
+        <f>IF(Sheet1!F290=0,Sheet1!C290&amp;",","")</f>
         <v/>
       </c>
       <c r="C283" t="str">
@@ -17580,7 +17579,7 @@
         <v/>
       </c>
       <c r="B284" t="str">
-        <f>IF(Sheet1!F291=0,","&amp;Sheet1!C291&amp;",","")</f>
+        <f>IF(Sheet1!F291=0,Sheet1!C291&amp;",","")</f>
         <v/>
       </c>
       <c r="C284" t="str">
@@ -17594,7 +17593,7 @@
         <v/>
       </c>
       <c r="B285" t="str">
-        <f>IF(Sheet1!F292=0,","&amp;Sheet1!C292&amp;",","")</f>
+        <f>IF(Sheet1!F292=0,Sheet1!C292&amp;",","")</f>
         <v/>
       </c>
       <c r="C285" t="str">
@@ -17608,7 +17607,7 @@
         <v/>
       </c>
       <c r="B286" t="str">
-        <f>IF(Sheet1!F293=0,","&amp;Sheet1!C293&amp;",","")</f>
+        <f>IF(Sheet1!F293=0,Sheet1!C293&amp;",","")</f>
         <v/>
       </c>
       <c r="C286" t="str">
@@ -17622,7 +17621,7 @@
         <v/>
       </c>
       <c r="B287" t="str">
-        <f>IF(Sheet1!F294=0,","&amp;Sheet1!C294&amp;",","")</f>
+        <f>IF(Sheet1!F294=0,Sheet1!C294&amp;",","")</f>
         <v/>
       </c>
       <c r="C287" t="str">
@@ -17636,7 +17635,7 @@
         <v/>
       </c>
       <c r="B288" t="str">
-        <f>IF(Sheet1!F295=0,","&amp;Sheet1!C295&amp;",","")</f>
+        <f>IF(Sheet1!F295=0,Sheet1!C295&amp;",","")</f>
         <v/>
       </c>
       <c r="C288" t="str">
@@ -17650,7 +17649,7 @@
         <v/>
       </c>
       <c r="B289" t="str">
-        <f>IF(Sheet1!F296=0,","&amp;Sheet1!C296&amp;",","")</f>
+        <f>IF(Sheet1!F296=0,Sheet1!C296&amp;",","")</f>
         <v/>
       </c>
       <c r="C289" t="str">
@@ -17664,7 +17663,7 @@
         <v/>
       </c>
       <c r="B290" t="str">
-        <f>IF(Sheet1!F297=0,","&amp;Sheet1!C297&amp;",","")</f>
+        <f>IF(Sheet1!F297=0,Sheet1!C297&amp;",","")</f>
         <v/>
       </c>
       <c r="C290" t="str">
@@ -17678,7 +17677,7 @@
         <v/>
       </c>
       <c r="B291" t="str">
-        <f>IF(Sheet1!F298=0,","&amp;Sheet1!C298&amp;",","")</f>
+        <f>IF(Sheet1!F298=0,Sheet1!C298&amp;",","")</f>
         <v/>
       </c>
       <c r="C291" t="str">
@@ -17692,7 +17691,7 @@
         <v/>
       </c>
       <c r="B292" t="str">
-        <f>IF(Sheet1!F299=0,","&amp;Sheet1!C299&amp;",","")</f>
+        <f>IF(Sheet1!F299=0,Sheet1!C299&amp;",","")</f>
         <v/>
       </c>
       <c r="C292" t="str">
@@ -17706,7 +17705,7 @@
         <v/>
       </c>
       <c r="B293" t="str">
-        <f>IF(Sheet1!F300=0,","&amp;Sheet1!C300&amp;",","")</f>
+        <f>IF(Sheet1!F300=0,Sheet1!C300&amp;",","")</f>
         <v/>
       </c>
       <c r="C293" t="str">
@@ -17720,7 +17719,7 @@
         <v/>
       </c>
       <c r="B294" t="str">
-        <f>IF(Sheet1!F301=0,","&amp;Sheet1!C301&amp;",","")</f>
+        <f>IF(Sheet1!F301=0,Sheet1!C301&amp;",","")</f>
         <v/>
       </c>
       <c r="C294" t="str">
@@ -17734,7 +17733,7 @@
         <v/>
       </c>
       <c r="B295" t="str">
-        <f>IF(Sheet1!F302=0,","&amp;Sheet1!C302&amp;",","")</f>
+        <f>IF(Sheet1!F302=0,Sheet1!C302&amp;",","")</f>
         <v/>
       </c>
       <c r="C295" t="str">
@@ -17748,7 +17747,7 @@
         <v/>
       </c>
       <c r="B296" t="str">
-        <f>IF(Sheet1!F303=0,","&amp;Sheet1!C303&amp;",","")</f>
+        <f>IF(Sheet1!F303=0,Sheet1!C303&amp;",","")</f>
         <v/>
       </c>
       <c r="C296" t="str">
@@ -17762,7 +17761,7 @@
         <v/>
       </c>
       <c r="B297" t="str">
-        <f>IF(Sheet1!F304=0,","&amp;Sheet1!C304&amp;",","")</f>
+        <f>IF(Sheet1!F304=0,Sheet1!C304&amp;",","")</f>
         <v/>
       </c>
       <c r="C297" t="str">
@@ -17776,7 +17775,7 @@
         <v/>
       </c>
       <c r="B298" t="str">
-        <f>IF(Sheet1!F305=0,","&amp;Sheet1!C305&amp;",","")</f>
+        <f>IF(Sheet1!F305=0,Sheet1!C305&amp;",","")</f>
         <v/>
       </c>
       <c r="C298" t="str">
@@ -17790,7 +17789,7 @@
         <v/>
       </c>
       <c r="B299" t="str">
-        <f>IF(Sheet1!F306=0,","&amp;Sheet1!C306&amp;",","")</f>
+        <f>IF(Sheet1!F306=0,Sheet1!C306&amp;",","")</f>
         <v/>
       </c>
       <c r="C299" t="str">
@@ -17804,7 +17803,7 @@
         <v/>
       </c>
       <c r="B300" t="str">
-        <f>IF(Sheet1!F307=0,","&amp;Sheet1!C307&amp;",","")</f>
+        <f>IF(Sheet1!F307=0,Sheet1!C307&amp;",","")</f>
         <v/>
       </c>
       <c r="C300" t="str">
@@ -17818,7 +17817,7 @@
         <v/>
       </c>
       <c r="B301" t="str">
-        <f>IF(Sheet1!F308=0,","&amp;Sheet1!C308&amp;",","")</f>
+        <f>IF(Sheet1!F308=0,Sheet1!C308&amp;",","")</f>
         <v/>
       </c>
       <c r="C301" t="str">
@@ -17832,7 +17831,7 @@
         <v/>
       </c>
       <c r="B302" t="str">
-        <f>IF(Sheet1!F309=0,","&amp;Sheet1!C309&amp;",","")</f>
+        <f>IF(Sheet1!F309=0,Sheet1!C309&amp;",","")</f>
         <v/>
       </c>
       <c r="C302" t="str">
@@ -17846,7 +17845,7 @@
         <v/>
       </c>
       <c r="B303" t="str">
-        <f>IF(Sheet1!F310=0,","&amp;Sheet1!C310&amp;",","")</f>
+        <f>IF(Sheet1!F310=0,Sheet1!C310&amp;",","")</f>
         <v/>
       </c>
       <c r="C303" t="str">
@@ -17860,8 +17859,8 @@
         <v>{,</v>
       </c>
       <c r="B304" t="str">
-        <f>IF(Sheet1!F311=0,","&amp;Sheet1!C311&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F311=0,Sheet1!C311&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
@@ -17870,8 +17869,8 @@
         <v>{,</v>
       </c>
       <c r="B305" t="str">
-        <f>IF(Sheet1!F312=0,","&amp;Sheet1!C312&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F312=0,Sheet1!C312&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
@@ -17880,8 +17879,8 @@
         <v>{,</v>
       </c>
       <c r="B306" t="str">
-        <f>IF(Sheet1!F313=0,","&amp;Sheet1!C313&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F313=0,Sheet1!C313&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
@@ -17890,8 +17889,8 @@
         <v>{,</v>
       </c>
       <c r="B307" t="str">
-        <f>IF(Sheet1!F314=0,","&amp;Sheet1!C314&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F314=0,Sheet1!C314&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
@@ -17900,8 +17899,8 @@
         <v>{,</v>
       </c>
       <c r="B308" t="str">
-        <f>IF(Sheet1!F315=0,","&amp;Sheet1!C315&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F315=0,Sheet1!C315&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
@@ -17910,8 +17909,8 @@
         <v>{,</v>
       </c>
       <c r="B309" t="str">
-        <f>IF(Sheet1!F316=0,","&amp;Sheet1!C316&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F316=0,Sheet1!C316&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
@@ -17920,8 +17919,8 @@
         <v>{,</v>
       </c>
       <c r="B310" t="str">
-        <f>IF(Sheet1!F317=0,","&amp;Sheet1!C317&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F317=0,Sheet1!C317&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
@@ -17930,8 +17929,8 @@
         <v>{,</v>
       </c>
       <c r="B311" t="str">
-        <f>IF(Sheet1!F318=0,","&amp;Sheet1!C318&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F318=0,Sheet1!C318&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
@@ -17940,8 +17939,8 @@
         <v>{,</v>
       </c>
       <c r="B312" t="str">
-        <f>IF(Sheet1!F319=0,","&amp;Sheet1!C319&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F319=0,Sheet1!C319&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
@@ -17950,8 +17949,8 @@
         <v>{,</v>
       </c>
       <c r="B313" t="str">
-        <f>IF(Sheet1!F320=0,","&amp;Sheet1!C320&amp;",",)</f>
-        <v>,,</v>
+        <f>IF(Sheet1!F320=0,Sheet1!C320&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
@@ -17959,791 +17958,1319 @@
         <f>IF(Sheet1!F321=0,"{"&amp;Sheet1!B321&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B314" t="str">
+        <f>IF(Sheet1!F321=0,Sheet1!C321&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="str">
         <f>IF(Sheet1!F322=0,"{"&amp;Sheet1!B322&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B315" t="str">
+        <f>IF(Sheet1!F322=0,Sheet1!C322&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="str">
         <f>IF(Sheet1!F323=0,"{"&amp;Sheet1!B323&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B316" t="str">
+        <f>IF(Sheet1!F323=0,Sheet1!C323&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="str">
         <f>IF(Sheet1!F324=0,"{"&amp;Sheet1!B324&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B317" t="str">
+        <f>IF(Sheet1!F324=0,Sheet1!C324&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="str">
         <f>IF(Sheet1!F325=0,"{"&amp;Sheet1!B325&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B318" t="str">
+        <f>IF(Sheet1!F325=0,Sheet1!C325&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="str">
         <f>IF(Sheet1!F326=0,"{"&amp;Sheet1!B326&amp;","," ")</f>
         <v>{,</v>
       </c>
+      <c r="B319" t="str">
+        <f>IF(Sheet1!F326=0,Sheet1!C326&amp;",","")</f>
+        <v>,</v>
+      </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="str">
         <f>IF(Sheet1!F327=0,"{"&amp;Sheet1!B327&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B320" t="str">
+        <f>IF(Sheet1!F327=0,Sheet1!C327&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="str">
         <f>IF(Sheet1!F328=0,"{"&amp;Sheet1!B328&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B321" t="str">
+        <f>IF(Sheet1!F328=0,Sheet1!C328&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="str">
         <f>IF(Sheet1!F329=0,"{"&amp;Sheet1!B329&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B322" t="str">
+        <f>IF(Sheet1!F329=0,Sheet1!C329&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="str">
         <f>IF(Sheet1!F330=0,"{"&amp;Sheet1!B330&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B323" t="str">
+        <f>IF(Sheet1!F330=0,Sheet1!C330&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="str">
         <f>IF(Sheet1!F331=0,"{"&amp;Sheet1!B331&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B324" t="str">
+        <f>IF(Sheet1!F331=0,Sheet1!C331&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="str">
         <f>IF(Sheet1!F332=0,"{"&amp;Sheet1!B332&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B325" t="str">
+        <f>IF(Sheet1!F332=0,Sheet1!C332&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="str">
         <f>IF(Sheet1!F333=0,"{"&amp;Sheet1!B333&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B326" t="str">
+        <f>IF(Sheet1!F333=0,Sheet1!C333&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="str">
         <f>IF(Sheet1!F334=0,"{"&amp;Sheet1!B334&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B327" t="str">
+        <f>IF(Sheet1!F334=0,Sheet1!C334&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="str">
         <f>IF(Sheet1!F335=0,"{"&amp;Sheet1!B335&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B328" t="str">
+        <f>IF(Sheet1!F335=0,Sheet1!C335&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="str">
         <f>IF(Sheet1!F336=0,"{"&amp;Sheet1!B336&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B329" t="str">
+        <f>IF(Sheet1!F336=0,Sheet1!C336&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="str">
         <f>IF(Sheet1!F337=0,"{"&amp;Sheet1!B337&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B330" t="str">
+        <f>IF(Sheet1!F337=0,Sheet1!C337&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="str">
         <f>IF(Sheet1!F338=0,"{"&amp;Sheet1!B338&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B331" t="str">
+        <f>IF(Sheet1!F338=0,Sheet1!C338&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="str">
         <f>IF(Sheet1!F339=0,"{"&amp;Sheet1!B339&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B332" t="str">
+        <f>IF(Sheet1!F339=0,Sheet1!C339&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="str">
         <f>IF(Sheet1!F340=0,"{"&amp;Sheet1!B340&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B333" t="str">
+        <f>IF(Sheet1!F340=0,Sheet1!C340&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="str">
         <f>IF(Sheet1!F341=0,"{"&amp;Sheet1!B341&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B334" t="str">
+        <f>IF(Sheet1!F341=0,Sheet1!C341&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="str">
         <f>IF(Sheet1!F342=0,"{"&amp;Sheet1!B342&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B335" t="str">
+        <f>IF(Sheet1!F342=0,Sheet1!C342&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="str">
         <f>IF(Sheet1!F343=0,"{"&amp;Sheet1!B343&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B336" t="str">
+        <f>IF(Sheet1!F343=0,Sheet1!C343&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="str">
         <f>IF(Sheet1!F344=0,"{"&amp;Sheet1!B344&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B337" t="str">
+        <f>IF(Sheet1!F344=0,Sheet1!C344&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="str">
         <f>IF(Sheet1!F345=0,"{"&amp;Sheet1!B345&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B338" t="str">
+        <f>IF(Sheet1!F345=0,Sheet1!C345&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="str">
         <f>IF(Sheet1!F346=0,"{"&amp;Sheet1!B346&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B339" t="str">
+        <f>IF(Sheet1!F346=0,Sheet1!C346&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="str">
         <f>IF(Sheet1!F347=0,"{"&amp;Sheet1!B347&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B340" t="str">
+        <f>IF(Sheet1!F347=0,Sheet1!C347&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="str">
         <f>IF(Sheet1!F348=0,"{"&amp;Sheet1!B348&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B341" t="str">
+        <f>IF(Sheet1!F348=0,Sheet1!C348&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="str">
         <f>IF(Sheet1!F349=0,"{"&amp;Sheet1!B349&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B342" t="str">
+        <f>IF(Sheet1!F349=0,Sheet1!C349&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="str">
         <f>IF(Sheet1!F350=0,"{"&amp;Sheet1!B350&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B343" t="str">
+        <f>IF(Sheet1!F350=0,Sheet1!C350&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="str">
         <f>IF(Sheet1!F351=0,"{"&amp;Sheet1!B351&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B344" t="str">
+        <f>IF(Sheet1!F351=0,Sheet1!C351&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="str">
         <f>IF(Sheet1!F352=0,"{"&amp;Sheet1!B352&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B345" t="str">
+        <f>IF(Sheet1!F352=0,Sheet1!C352&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="str">
         <f>IF(Sheet1!F353=0,"{"&amp;Sheet1!B353&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B346" t="str">
+        <f>IF(Sheet1!F353=0,Sheet1!C353&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="str">
         <f>IF(Sheet1!F354=0,"{"&amp;Sheet1!B354&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B347" t="str">
+        <f>IF(Sheet1!F354=0,Sheet1!C354&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="str">
         <f>IF(Sheet1!F355=0,"{"&amp;Sheet1!B355&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B348" t="str">
+        <f>IF(Sheet1!F355=0,Sheet1!C355&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="str">
         <f>IF(Sheet1!F356=0,"{"&amp;Sheet1!B356&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B349" t="str">
+        <f>IF(Sheet1!F356=0,Sheet1!C356&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" t="str">
         <f>IF(Sheet1!F357=0,"{"&amp;Sheet1!B357&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B350" t="str">
+        <f>IF(Sheet1!F357=0,Sheet1!C357&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="str">
         <f>IF(Sheet1!F358=0,"{"&amp;Sheet1!B358&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B351" t="str">
+        <f>IF(Sheet1!F358=0,Sheet1!C358&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="str">
         <f>IF(Sheet1!F359=0,"{"&amp;Sheet1!B359&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B352" t="str">
+        <f>IF(Sheet1!F359=0,Sheet1!C359&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="str">
         <f>IF(Sheet1!F360=0,"{"&amp;Sheet1!B360&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B353" t="str">
+        <f>IF(Sheet1!F360=0,Sheet1!C360&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" t="str">
         <f>IF(Sheet1!F361=0,"{"&amp;Sheet1!B361&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B354" t="str">
+        <f>IF(Sheet1!F361=0,Sheet1!C361&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="str">
         <f>IF(Sheet1!F362=0,"{"&amp;Sheet1!B362&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B355" t="str">
+        <f>IF(Sheet1!F362=0,Sheet1!C362&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="str">
         <f>IF(Sheet1!F363=0,"{"&amp;Sheet1!B363&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B356" t="str">
+        <f>IF(Sheet1!F363=0,Sheet1!C363&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="str">
         <f>IF(Sheet1!F364=0,"{"&amp;Sheet1!B364&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B357" t="str">
+        <f>IF(Sheet1!F364=0,Sheet1!C364&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="str">
         <f>IF(Sheet1!F365=0,"{"&amp;Sheet1!B365&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B358" t="str">
+        <f>IF(Sheet1!F365=0,Sheet1!C365&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="str">
         <f>IF(Sheet1!F366=0,"{"&amp;Sheet1!B366&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B359" t="str">
+        <f>IF(Sheet1!F366=0,Sheet1!C366&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="str">
         <f>IF(Sheet1!F367=0,"{"&amp;Sheet1!B367&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B360" t="str">
+        <f>IF(Sheet1!F367=0,Sheet1!C367&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="str">
         <f>IF(Sheet1!F368=0,"{"&amp;Sheet1!B368&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B361" t="str">
+        <f>IF(Sheet1!F368=0,Sheet1!C368&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="str">
         <f>IF(Sheet1!F369=0,"{"&amp;Sheet1!B369&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B362" t="str">
+        <f>IF(Sheet1!F369=0,Sheet1!C369&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="str">
         <f>IF(Sheet1!F370=0,"{"&amp;Sheet1!B370&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B363" t="str">
+        <f>IF(Sheet1!F370=0,Sheet1!C370&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="str">
         <f>IF(Sheet1!F371=0,"{"&amp;Sheet1!B371&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B364" t="str">
+        <f>IF(Sheet1!F371=0,Sheet1!C371&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="str">
         <f>IF(Sheet1!F372=0,"{"&amp;Sheet1!B372&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B365" t="str">
+        <f>IF(Sheet1!F372=0,Sheet1!C372&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="str">
         <f>IF(Sheet1!F373=0,"{"&amp;Sheet1!B373&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B366" t="str">
+        <f>IF(Sheet1!F373=0,Sheet1!C373&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="str">
         <f>IF(Sheet1!F374=0,"{"&amp;Sheet1!B374&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B367" t="str">
+        <f>IF(Sheet1!F374=0,Sheet1!C374&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="str">
         <f>IF(Sheet1!F375=0,"{"&amp;Sheet1!B375&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B368" t="str">
+        <f>IF(Sheet1!F375=0,Sheet1!C375&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="str">
         <f>IF(Sheet1!F376=0,"{"&amp;Sheet1!B376&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B369" t="str">
+        <f>IF(Sheet1!F376=0,Sheet1!C376&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="str">
         <f>IF(Sheet1!F377=0,"{"&amp;Sheet1!B377&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B370" t="str">
+        <f>IF(Sheet1!F377=0,Sheet1!C377&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="str">
         <f>IF(Sheet1!F378=0,"{"&amp;Sheet1!B378&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B371" t="str">
+        <f>IF(Sheet1!F378=0,Sheet1!C378&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="str">
         <f>IF(Sheet1!F379=0,"{"&amp;Sheet1!B379&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B372" t="str">
+        <f>IF(Sheet1!F379=0,Sheet1!C379&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="str">
         <f>IF(Sheet1!F380=0,"{"&amp;Sheet1!B380&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B373" t="str">
+        <f>IF(Sheet1!F380=0,Sheet1!C380&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="str">
         <f>IF(Sheet1!F381=0,"{"&amp;Sheet1!B381&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B374" t="str">
+        <f>IF(Sheet1!F381=0,Sheet1!C381&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="str">
         <f>IF(Sheet1!F382=0,"{"&amp;Sheet1!B382&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B375" t="str">
+        <f>IF(Sheet1!F382=0,Sheet1!C382&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="str">
         <f>IF(Sheet1!F383=0,"{"&amp;Sheet1!B383&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B376" t="str">
+        <f>IF(Sheet1!F383=0,Sheet1!C383&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="str">
         <f>IF(Sheet1!F384=0,"{"&amp;Sheet1!B384&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B377" t="str">
+        <f>IF(Sheet1!F384=0,Sheet1!C384&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="str">
         <f>IF(Sheet1!F385=0,"{"&amp;Sheet1!B385&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B378" t="str">
+        <f>IF(Sheet1!F385=0,Sheet1!C385&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="str">
         <f>IF(Sheet1!F386=0,"{"&amp;Sheet1!B386&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B379" t="str">
+        <f>IF(Sheet1!F386=0,Sheet1!C386&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="str">
         <f>IF(Sheet1!F387=0,"{"&amp;Sheet1!B387&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B380" t="str">
+        <f>IF(Sheet1!F387=0,Sheet1!C387&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="str">
         <f>IF(Sheet1!F388=0,"{"&amp;Sheet1!B388&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B381" t="str">
+        <f>IF(Sheet1!F388=0,Sheet1!C388&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="str">
         <f>IF(Sheet1!F389=0,"{"&amp;Sheet1!B389&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B382" t="str">
+        <f>IF(Sheet1!F389=0,Sheet1!C389&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="str">
         <f>IF(Sheet1!F390=0,"{"&amp;Sheet1!B390&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B383" t="str">
+        <f>IF(Sheet1!F390=0,Sheet1!C390&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="str">
         <f>IF(Sheet1!F391=0,"{"&amp;Sheet1!B391&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B384" t="str">
+        <f>IF(Sheet1!F391=0,Sheet1!C391&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="str">
         <f>IF(Sheet1!F392=0,"{"&amp;Sheet1!B392&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B385" t="str">
+        <f>IF(Sheet1!F392=0,Sheet1!C392&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="str">
         <f>IF(Sheet1!F393=0,"{"&amp;Sheet1!B393&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B386" t="str">
+        <f>IF(Sheet1!F393=0,Sheet1!C393&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="str">
         <f>IF(Sheet1!F394=0,"{"&amp;Sheet1!B394&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B387" t="str">
+        <f>IF(Sheet1!F394=0,Sheet1!C394&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="str">
         <f>IF(Sheet1!F395=0,"{"&amp;Sheet1!B395&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B388" t="str">
+        <f>IF(Sheet1!F395=0,Sheet1!C395&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="str">
         <f>IF(Sheet1!F396=0,"{"&amp;Sheet1!B396&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B389" t="str">
+        <f>IF(Sheet1!F396=0,Sheet1!C396&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="str">
         <f>IF(Sheet1!F397=0,"{"&amp;Sheet1!B397&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B390" t="str">
+        <f>IF(Sheet1!F397=0,Sheet1!C397&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="str">
         <f>IF(Sheet1!F398=0,"{"&amp;Sheet1!B398&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B391" t="str">
+        <f>IF(Sheet1!F398=0,Sheet1!C398&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="str">
         <f>IF(Sheet1!F399=0,"{"&amp;Sheet1!B399&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B392" t="str">
+        <f>IF(Sheet1!F399=0,Sheet1!C399&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="str">
         <f>IF(Sheet1!F400=0,"{"&amp;Sheet1!B400&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B393" t="str">
+        <f>IF(Sheet1!F400=0,Sheet1!C400&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="str">
         <f>IF(Sheet1!F401=0,"{"&amp;Sheet1!B401&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B394" t="str">
+        <f>IF(Sheet1!F401=0,Sheet1!C401&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="str">
         <f>IF(Sheet1!F402=0,"{"&amp;Sheet1!B402&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B395" t="str">
+        <f>IF(Sheet1!F402=0,Sheet1!C402&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="str">
         <f>IF(Sheet1!F403=0,"{"&amp;Sheet1!B403&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B396" t="str">
+        <f>IF(Sheet1!F403=0,Sheet1!C403&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="str">
         <f>IF(Sheet1!F404=0,"{"&amp;Sheet1!B404&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B397" t="str">
+        <f>IF(Sheet1!F404=0,Sheet1!C404&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="str">
         <f>IF(Sheet1!F405=0,"{"&amp;Sheet1!B405&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B398" t="str">
+        <f>IF(Sheet1!F405=0,Sheet1!C405&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="str">
         <f>IF(Sheet1!F406=0,"{"&amp;Sheet1!B406&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B399" t="str">
+        <f>IF(Sheet1!F406=0,Sheet1!C406&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="str">
         <f>IF(Sheet1!F407=0,"{"&amp;Sheet1!B407&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B400" t="str">
+        <f>IF(Sheet1!F407=0,Sheet1!C407&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="str">
         <f>IF(Sheet1!F408=0,"{"&amp;Sheet1!B408&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B401" t="str">
+        <f>IF(Sheet1!F408=0,Sheet1!C408&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="str">
         <f>IF(Sheet1!F409=0,"{"&amp;Sheet1!B409&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B402" t="str">
+        <f>IF(Sheet1!F409=0,Sheet1!C409&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" t="str">
         <f>IF(Sheet1!F410=0,"{"&amp;Sheet1!B410&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B403" t="str">
+        <f>IF(Sheet1!F410=0,Sheet1!C410&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="str">
         <f>IF(Sheet1!F411=0,"{"&amp;Sheet1!B411&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B404" t="str">
+        <f>IF(Sheet1!F411=0,Sheet1!C411&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="str">
         <f>IF(Sheet1!F412=0,"{"&amp;Sheet1!B412&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B405" t="str">
+        <f>IF(Sheet1!F412=0,Sheet1!C412&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="str">
         <f>IF(Sheet1!F413=0,"{"&amp;Sheet1!B413&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B406" t="str">
+        <f>IF(Sheet1!F413=0,Sheet1!C413&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="str">
         <f>IF(Sheet1!F414=0,"{"&amp;Sheet1!B414&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B407" t="str">
+        <f>IF(Sheet1!F414=0,Sheet1!C414&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" t="str">
         <f>IF(Sheet1!F415=0,"{"&amp;Sheet1!B415&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B408" t="str">
+        <f>IF(Sheet1!F415=0,Sheet1!C415&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" t="str">
         <f>IF(Sheet1!F416=0,"{"&amp;Sheet1!B416&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B409" t="str">
+        <f>IF(Sheet1!F416=0,Sheet1!C416&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" t="str">
         <f>IF(Sheet1!F417=0,"{"&amp;Sheet1!B417&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B410" t="str">
+        <f>IF(Sheet1!F417=0,Sheet1!C417&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" t="str">
         <f>IF(Sheet1!F418=0,"{"&amp;Sheet1!B418&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B411" t="str">
+        <f>IF(Sheet1!F418=0,Sheet1!C418&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" t="str">
         <f>IF(Sheet1!F419=0,"{"&amp;Sheet1!B419&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B412" t="str">
+        <f>IF(Sheet1!F419=0,Sheet1!C419&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" t="str">
         <f>IF(Sheet1!F420=0,"{"&amp;Sheet1!B420&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B413" t="str">
+        <f>IF(Sheet1!F420=0,Sheet1!C420&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" t="str">
         <f>IF(Sheet1!F421=0,"{"&amp;Sheet1!B421&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B414" t="str">
+        <f>IF(Sheet1!F421=0,Sheet1!C421&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" t="str">
         <f>IF(Sheet1!F422=0,"{"&amp;Sheet1!B422&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B415" t="str">
+        <f>IF(Sheet1!F422=0,Sheet1!C422&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" t="str">
         <f>IF(Sheet1!F423=0,"{"&amp;Sheet1!B423&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B416" t="str">
+        <f>IF(Sheet1!F423=0,Sheet1!C423&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="str">
         <f>IF(Sheet1!F424=0,"{"&amp;Sheet1!B424&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B417" t="str">
+        <f>IF(Sheet1!F424=0,Sheet1!C424&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="str">
         <f>IF(Sheet1!F425=0,"{"&amp;Sheet1!B425&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B418" t="str">
+        <f>IF(Sheet1!F425=0,Sheet1!C425&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="str">
         <f>IF(Sheet1!F426=0,"{"&amp;Sheet1!B426&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B419" t="str">
+        <f>IF(Sheet1!F426=0,Sheet1!C426&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="str">
         <f>IF(Sheet1!F427=0,"{"&amp;Sheet1!B427&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B420" t="str">
+        <f>IF(Sheet1!F427=0,Sheet1!C427&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="str">
         <f>IF(Sheet1!F428=0,"{"&amp;Sheet1!B428&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B421" t="str">
+        <f>IF(Sheet1!F428=0,Sheet1!C428&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" t="str">
         <f>IF(Sheet1!F429=0,"{"&amp;Sheet1!B429&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B422" t="str">
+        <f>IF(Sheet1!F429=0,Sheet1!C429&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="str">
         <f>IF(Sheet1!F430=0,"{"&amp;Sheet1!B430&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B423" t="str">
+        <f>IF(Sheet1!F430=0,Sheet1!C430&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="str">
         <f>IF(Sheet1!F431=0,"{"&amp;Sheet1!B431&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B424" t="str">
+        <f>IF(Sheet1!F431=0,Sheet1!C431&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" t="str">
         <f>IF(Sheet1!F432=0,"{"&amp;Sheet1!B432&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B425" t="str">
+        <f>IF(Sheet1!F432=0,Sheet1!C432&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" t="str">
         <f>IF(Sheet1!F433=0,"{"&amp;Sheet1!B433&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B426" t="str">
+        <f>IF(Sheet1!F433=0,Sheet1!C433&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" t="str">
         <f>IF(Sheet1!F434=0,"{"&amp;Sheet1!B434&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B427" t="str">
+        <f>IF(Sheet1!F434=0,Sheet1!C434&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" t="str">
         <f>IF(Sheet1!F435=0,"{"&amp;Sheet1!B435&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B428" t="str">
+        <f>IF(Sheet1!F435=0,Sheet1!C435&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" t="str">
         <f>IF(Sheet1!F436=0,"{"&amp;Sheet1!B436&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B429" t="str">
+        <f>IF(Sheet1!F436=0,Sheet1!C436&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" t="str">
         <f>IF(Sheet1!F437=0,"{"&amp;Sheet1!B437&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B430" t="str">
+        <f>IF(Sheet1!F437=0,Sheet1!C437&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="str">
         <f>IF(Sheet1!F438=0,"{"&amp;Sheet1!B438&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B431" t="str">
+        <f>IF(Sheet1!F438=0,Sheet1!C438&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="str">
         <f>IF(Sheet1!F439=0,"{"&amp;Sheet1!B439&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B432" t="str">
+        <f>IF(Sheet1!F439=0,Sheet1!C439&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="str">
         <f>IF(Sheet1!F440=0,"{"&amp;Sheet1!B440&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B433" t="str">
+        <f>IF(Sheet1!F440=0,Sheet1!C440&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="str">
         <f>IF(Sheet1!F441=0,"{"&amp;Sheet1!B441&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B434" t="str">
+        <f>IF(Sheet1!F441=0,Sheet1!C441&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="str">
         <f>IF(Sheet1!F442=0,"{"&amp;Sheet1!B442&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B435" t="str">
+        <f>IF(Sheet1!F442=0,Sheet1!C442&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="str">
         <f>IF(Sheet1!F443=0,"{"&amp;Sheet1!B443&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B436" t="str">
+        <f>IF(Sheet1!F443=0,Sheet1!C443&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="str">
         <f>IF(Sheet1!F444=0,"{"&amp;Sheet1!B444&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B437" t="str">
+        <f>IF(Sheet1!F444=0,Sheet1!C444&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="str">
         <f>IF(Sheet1!F445=0,"{"&amp;Sheet1!B445&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B438" t="str">
+        <f>IF(Sheet1!F445=0,Sheet1!C445&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" t="str">
         <f>IF(Sheet1!F446=0,"{"&amp;Sheet1!B446&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B439" t="str">
+        <f>IF(Sheet1!F446=0,Sheet1!C446&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="str">
         <f>IF(Sheet1!F447=0,"{"&amp;Sheet1!B447&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B440" t="str">
+        <f>IF(Sheet1!F447=0,Sheet1!C447&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="str">
         <f>IF(Sheet1!F448=0,"{"&amp;Sheet1!B448&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B441" t="str">
+        <f>IF(Sheet1!F448=0,Sheet1!C448&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="str">
         <f>IF(Sheet1!F449=0,"{"&amp;Sheet1!B449&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B442" t="str">
+        <f>IF(Sheet1!F449=0,Sheet1!C449&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="str">
         <f>IF(Sheet1!F450=0,"{"&amp;Sheet1!B450&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B443" t="str">
+        <f>IF(Sheet1!F450=0,Sheet1!C450&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" t="str">
         <f>IF(Sheet1!F451=0,"{"&amp;Sheet1!B451&amp;","," ")</f>
         <v>{,</v>
       </c>
-    </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B444" t="str">
+        <f>IF(Sheet1!F451=0,Sheet1!C451&amp;",","")</f>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" t="str">
         <f>IF(Sheet1!F452=0,"{"&amp;Sheet1!B452&amp;","," ")</f>
         <v>{,</v>
+      </c>
+      <c r="B445" t="str">
+        <f>IF(Sheet1!F452=0,Sheet1!C452&amp;",","")</f>
+        <v>,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>